<commit_message>
Edited sprint backlog to current work.
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/170ad8df2ec9dbaf/Ambiente de Trabalho/Nova pasta/SE2122_57464_58763_57677_58125_63764/scrum/Phase1/Sprint1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{ACC44164-E8E0-4451-AA09-2BE7526D8755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E0EA1CA-3CDD-4B36-894B-E73C23173EB8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F180C23-822B-45D3-9D5F-E2F2D085601F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1056" yWindow="-108" windowWidth="22092" windowHeight="13176" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,8 @@
   </si>
   <si>
     <t>Member 2: detecting smells
-Member 1: detecting smells</t>
+Member 1: detecting smells
+Member 5: detecting smells</t>
   </si>
 </sst>
 </file>
@@ -198,25 +199,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -227,6 +216,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -547,7 +548,7 @@
   <dimension ref="A1:AL161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F6"/>
+      <selection activeCell="G7" sqref="G7:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,26 +599,26 @@
       <c r="AL1" s="2"/>
     </row>
     <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -650,19 +651,19 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -690,18 +691,18 @@
       <c r="AK3" s="2"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -729,18 +730,18 @@
       <c r="AK4" s="2"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -768,18 +769,18 @@
       <c r="AK5" s="2"/>
     </row>
     <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -812,17 +813,17 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -850,18 +851,18 @@
       <c r="AK7" s="2"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -889,18 +890,18 @@
       <c r="AK8" s="2"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -928,18 +929,18 @@
       <c r="AK9" s="2"/>
     </row>
     <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -967,22 +968,22 @@
       <c r="AK10" s="2"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="10" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1010,18 +1011,18 @@
       <c r="AK11" s="2"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1049,18 +1050,18 @@
       <c r="AK12" s="2"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1088,18 +1089,18 @@
       <c r="AK13" s="2"/>
     </row>
     <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1127,22 +1128,22 @@
       <c r="AK14" s="2"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1170,18 +1171,18 @@
       <c r="AK15" s="2"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1209,18 +1210,18 @@
       <c r="AK16" s="2"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1248,18 +1249,18 @@
       <c r="AK17" s="2"/>
     </row>
     <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -5149,6 +5150,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A15:C18"/>
     <mergeCell ref="D15:F18"/>
     <mergeCell ref="G15:I18"/>
@@ -5162,19 +5170,21 @@
     <mergeCell ref="D11:F14"/>
     <mergeCell ref="G11:I14"/>
     <mergeCell ref="J11:L14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008EA8F6205B617B4CBD762DBD6D300502" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="000a41c94a85e4495c2f2d3453c30ed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10b95d85-a823-4616-89f6-0a6587d88b0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0729d4038857d2ede91d1e28869f4e90" ns3:_="">
     <xsd:import namespace="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
@@ -5320,15 +5330,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5336,6 +5337,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A39B317-7C09-4361-8F9C-EC6B55EB4D12}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5349,14 +5358,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
sprint backlog update member 2
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Faculdade\3º Ano\1º Semestre\ES\jabref\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790FE152-0A66-4FAA-A378-9A3EAF51F112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5261CF4-1385-4C81-AA46-B33C47890F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
@@ -75,10 +75,12 @@
 Member 5: detecting smells</t>
   </si>
   <si>
-    <t>Member 5: finished code smells.</t>
+    <t>Member 5: finished code smells.
+Member 2: finished code smells.</t>
   </si>
   <si>
-    <t>Member 5: detecting patterns.</t>
+    <t>Member 5: detecting patterns.
+Member 2: detecting patterns.</t>
   </si>
 </sst>
 </file>
@@ -197,7 +199,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -205,13 +207,25 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -223,20 +237,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -556,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0899AEA-CFD5-4FE7-96CD-5876EC28C07C}">
   <dimension ref="A1:AL161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,26 +614,26 @@
       <c r="AL1" s="2"/>
     </row>
     <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="12" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -661,12 +666,12 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="7"/>
@@ -674,8 +679,8 @@
       <c r="J3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -703,18 +708,18 @@
       <c r="AK3" s="2"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -742,18 +747,18 @@
       <c r="AK4" s="2"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -781,18 +786,18 @@
       <c r="AK5" s="2"/>
     </row>
     <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -825,17 +830,17 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -863,18 +868,18 @@
       <c r="AK7" s="2"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -902,18 +907,18 @@
       <c r="AK8" s="2"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -941,18 +946,18 @@
       <c r="AK9" s="2"/>
     </row>
     <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -980,24 +985,24 @@
       <c r="AK10" s="2"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1025,18 +1030,18 @@
       <c r="AK11" s="2"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1064,18 +1069,18 @@
       <c r="AK12" s="2"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1103,18 +1108,18 @@
       <c r="AK13" s="2"/>
     </row>
     <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1142,22 +1147,22 @@
       <c r="AK14" s="2"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1185,18 +1190,18 @@
       <c r="AK15" s="2"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1224,18 +1229,18 @@
       <c r="AK16" s="2"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1263,18 +1268,18 @@
       <c r="AK17" s="2"/>
     </row>
     <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -5164,13 +5169,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A15:C18"/>
     <mergeCell ref="D15:F18"/>
     <mergeCell ref="G15:I18"/>
@@ -5184,6 +5182,13 @@
     <mergeCell ref="D11:F14"/>
     <mergeCell ref="G11:I14"/>
     <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5191,15 +5196,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008EA8F6205B617B4CBD762DBD6D300502" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="000a41c94a85e4495c2f2d3453c30ed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10b95d85-a823-4616-89f6-0a6587d88b0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0729d4038857d2ede91d1e28869f4e90" ns3:_="">
     <xsd:import namespace="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
@@ -5345,6 +5341,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5352,14 +5357,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A39B317-7C09-4361-8F9C-EC6B55EB4D12}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5373,6 +5370,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Team member 1: atualizei o backlog
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nova pasta\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27F7E70-5CAD-4F14-9318-6F3817AE5C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C49D03-8DB8-46AA-953C-23C47237491C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -89,12 +89,13 @@
 Member 1: detecting patterns.</t>
   </si>
   <si>
-    <t>Member 5: finished patterns.</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Member 1: Doing the metrics
 Member 5: Doing the metrics</t>
+  </si>
+  <si>
+    <t>Member 5: finished patterns.
+Member 1: finished patterns.</t>
   </si>
 </sst>
 </file>
@@ -221,25 +222,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -255,6 +244,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -576,16 +577,16 @@
   <dimension ref="A1:AL161"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:I10"/>
+      <selection activeCell="J11" sqref="J11:L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="46.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -627,27 +628,27 @@
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
     </row>
-    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -674,27 +675,27 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -721,19 +722,19 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -760,19 +761,19 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -799,19 +800,19 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
+    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -838,23 +839,23 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -881,19 +882,19 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -920,19 +921,19 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -959,19 +960,19 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -998,27 +999,27 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="10" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11" t="s">
-        <v>14</v>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="8" t="s">
+        <v>15</v>
       </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1045,19 +1046,19 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1084,19 +1085,19 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1123,19 +1124,19 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1162,25 +1163,25 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="12" t="s">
-        <v>15</v>
+      <c r="G15" s="8" t="s">
+        <v>14</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1207,19 +1208,19 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1246,19 +1247,19 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1285,19 +1286,19 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
-    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
+    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1324,7 +1325,7 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1351,7 +1352,7 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1378,7 +1379,7 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -1405,7 +1406,7 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -1432,7 +1433,7 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1459,7 +1460,7 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1486,7 +1487,7 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -1513,7 +1514,7 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -1540,7 +1541,7 @@
       <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1567,7 +1568,7 @@
       <c r="AJ27" s="2"/>
       <c r="AK27" s="2"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -1594,7 +1595,7 @@
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -1621,7 +1622,7 @@
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -1648,7 +1649,7 @@
       <c r="AJ30" s="2"/>
       <c r="AK30" s="2"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -1675,7 +1676,7 @@
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -1702,7 +1703,7 @@
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
     </row>
-    <row r="33" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -1729,7 +1730,7 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
     </row>
-    <row r="34" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -1756,7 +1757,7 @@
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
     </row>
-    <row r="35" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -1783,7 +1784,7 @@
       <c r="AJ35" s="2"/>
       <c r="AK35" s="2"/>
     </row>
-    <row r="36" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -1810,7 +1811,7 @@
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
     </row>
-    <row r="37" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -1837,7 +1838,7 @@
       <c r="AJ37" s="2"/>
       <c r="AK37" s="2"/>
     </row>
-    <row r="38" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -1864,7 +1865,7 @@
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
     </row>
-    <row r="39" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -1891,7 +1892,7 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
     </row>
-    <row r="40" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -1918,7 +1919,7 @@
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
     </row>
-    <row r="41" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -1945,7 +1946,7 @@
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
     </row>
-    <row r="42" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -1972,7 +1973,7 @@
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
     </row>
-    <row r="43" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -1999,7 +2000,7 @@
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
     </row>
-    <row r="44" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -2026,7 +2027,7 @@
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
     </row>
-    <row r="45" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -2053,7 +2054,7 @@
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
     </row>
-    <row r="46" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -2080,7 +2081,7 @@
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
     </row>
-    <row r="47" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -2107,7 +2108,7 @@
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
     </row>
-    <row r="48" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -2134,7 +2135,7 @@
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
     </row>
-    <row r="49" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -2161,7 +2162,7 @@
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2"/>
     </row>
-    <row r="50" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -2188,7 +2189,7 @@
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
     </row>
-    <row r="51" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -2215,7 +2216,7 @@
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
     </row>
-    <row r="52" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -2242,7 +2243,7 @@
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
     </row>
-    <row r="53" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -2269,7 +2270,7 @@
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
     </row>
-    <row r="54" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -2296,7 +2297,7 @@
       <c r="AJ54" s="2"/>
       <c r="AK54" s="2"/>
     </row>
-    <row r="55" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -2323,7 +2324,7 @@
       <c r="AJ55" s="2"/>
       <c r="AK55" s="2"/>
     </row>
-    <row r="56" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -2350,7 +2351,7 @@
       <c r="AJ56" s="2"/>
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -2377,7 +2378,7 @@
       <c r="AJ57" s="2"/>
       <c r="AK57" s="2"/>
     </row>
-    <row r="58" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -2404,7 +2405,7 @@
       <c r="AJ58" s="2"/>
       <c r="AK58" s="2"/>
     </row>
-    <row r="59" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -2431,7 +2432,7 @@
       <c r="AJ59" s="2"/>
       <c r="AK59" s="2"/>
     </row>
-    <row r="60" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -2458,7 +2459,7 @@
       <c r="AJ60" s="2"/>
       <c r="AK60" s="2"/>
     </row>
-    <row r="61" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -2485,7 +2486,7 @@
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
     </row>
-    <row r="62" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -2512,7 +2513,7 @@
       <c r="AJ62" s="2"/>
       <c r="AK62" s="2"/>
     </row>
-    <row r="63" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -2539,7 +2540,7 @@
       <c r="AJ63" s="2"/>
       <c r="AK63" s="2"/>
     </row>
-    <row r="64" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -2566,7 +2567,7 @@
       <c r="AJ64" s="2"/>
       <c r="AK64" s="2"/>
     </row>
-    <row r="65" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
@@ -2593,7 +2594,7 @@
       <c r="AJ65" s="2"/>
       <c r="AK65" s="2"/>
     </row>
-    <row r="66" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -2620,7 +2621,7 @@
       <c r="AJ66" s="2"/>
       <c r="AK66" s="2"/>
     </row>
-    <row r="67" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -2647,7 +2648,7 @@
       <c r="AJ67" s="2"/>
       <c r="AK67" s="2"/>
     </row>
-    <row r="68" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -2674,7 +2675,7 @@
       <c r="AJ68" s="2"/>
       <c r="AK68" s="2"/>
     </row>
-    <row r="69" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -2701,7 +2702,7 @@
       <c r="AJ69" s="2"/>
       <c r="AK69" s="2"/>
     </row>
-    <row r="70" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
@@ -2728,7 +2729,7 @@
       <c r="AJ70" s="2"/>
       <c r="AK70" s="2"/>
     </row>
-    <row r="71" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
@@ -2755,7 +2756,7 @@
       <c r="AJ71" s="2"/>
       <c r="AK71" s="2"/>
     </row>
-    <row r="72" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
@@ -2782,7 +2783,7 @@
       <c r="AJ72" s="2"/>
       <c r="AK72" s="2"/>
     </row>
-    <row r="73" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -2809,7 +2810,7 @@
       <c r="AJ73" s="2"/>
       <c r="AK73" s="2"/>
     </row>
-    <row r="74" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
@@ -2836,7 +2837,7 @@
       <c r="AJ74" s="2"/>
       <c r="AK74" s="2"/>
     </row>
-    <row r="75" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="75" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -2863,7 +2864,7 @@
       <c r="AJ75" s="2"/>
       <c r="AK75" s="2"/>
     </row>
-    <row r="76" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="76" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -2890,7 +2891,7 @@
       <c r="AJ76" s="2"/>
       <c r="AK76" s="2"/>
     </row>
-    <row r="77" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="77" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -2917,7 +2918,7 @@
       <c r="AJ77" s="2"/>
       <c r="AK77" s="2"/>
     </row>
-    <row r="78" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="78" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -2944,7 +2945,7 @@
       <c r="AJ78" s="2"/>
       <c r="AK78" s="2"/>
     </row>
-    <row r="79" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="79" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -2971,7 +2972,7 @@
       <c r="AJ79" s="2"/>
       <c r="AK79" s="2"/>
     </row>
-    <row r="80" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="80" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
@@ -2998,7 +2999,7 @@
       <c r="AJ80" s="2"/>
       <c r="AK80" s="2"/>
     </row>
-    <row r="81" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="81" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
@@ -3025,7 +3026,7 @@
       <c r="AJ81" s="2"/>
       <c r="AK81" s="2"/>
     </row>
-    <row r="82" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="82" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
@@ -3052,7 +3053,7 @@
       <c r="AJ82" s="2"/>
       <c r="AK82" s="2"/>
     </row>
-    <row r="83" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="83" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
@@ -3079,7 +3080,7 @@
       <c r="AJ83" s="2"/>
       <c r="AK83" s="2"/>
     </row>
-    <row r="84" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="84" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
@@ -3106,7 +3107,7 @@
       <c r="AJ84" s="2"/>
       <c r="AK84" s="2"/>
     </row>
-    <row r="85" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="85" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
@@ -3133,7 +3134,7 @@
       <c r="AJ85" s="2"/>
       <c r="AK85" s="2"/>
     </row>
-    <row r="86" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="86" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -3160,7 +3161,7 @@
       <c r="AJ86" s="2"/>
       <c r="AK86" s="2"/>
     </row>
-    <row r="87" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="87" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
@@ -3187,7 +3188,7 @@
       <c r="AJ87" s="2"/>
       <c r="AK87" s="2"/>
     </row>
-    <row r="88" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="88" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -3214,7 +3215,7 @@
       <c r="AJ88" s="2"/>
       <c r="AK88" s="2"/>
     </row>
-    <row r="89" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="89" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
@@ -3241,7 +3242,7 @@
       <c r="AJ89" s="2"/>
       <c r="AK89" s="2"/>
     </row>
-    <row r="90" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="90" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
@@ -3268,7 +3269,7 @@
       <c r="AJ90" s="2"/>
       <c r="AK90" s="2"/>
     </row>
-    <row r="91" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="91" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
@@ -3295,7 +3296,7 @@
       <c r="AJ91" s="2"/>
       <c r="AK91" s="2"/>
     </row>
-    <row r="92" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="92" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -3322,7 +3323,7 @@
       <c r="AJ92" s="2"/>
       <c r="AK92" s="2"/>
     </row>
-    <row r="93" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="93" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -3349,7 +3350,7 @@
       <c r="AJ93" s="2"/>
       <c r="AK93" s="2"/>
     </row>
-    <row r="94" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="94" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
@@ -3376,7 +3377,7 @@
       <c r="AJ94" s="2"/>
       <c r="AK94" s="2"/>
     </row>
-    <row r="95" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="95" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
@@ -3403,7 +3404,7 @@
       <c r="AJ95" s="2"/>
       <c r="AK95" s="2"/>
     </row>
-    <row r="96" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="96" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -3430,7 +3431,7 @@
       <c r="AJ96" s="2"/>
       <c r="AK96" s="2"/>
     </row>
-    <row r="97" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="97" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -3457,7 +3458,7 @@
       <c r="AJ97" s="2"/>
       <c r="AK97" s="2"/>
     </row>
-    <row r="98" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
@@ -3484,7 +3485,7 @@
       <c r="AJ98" s="2"/>
       <c r="AK98" s="2"/>
     </row>
-    <row r="99" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="99" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
@@ -3511,7 +3512,7 @@
       <c r="AJ99" s="2"/>
       <c r="AK99" s="2"/>
     </row>
-    <row r="100" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="100" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
@@ -3538,7 +3539,7 @@
       <c r="AJ100" s="2"/>
       <c r="AK100" s="2"/>
     </row>
-    <row r="101" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="101" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
@@ -3565,7 +3566,7 @@
       <c r="AJ101" s="2"/>
       <c r="AK101" s="2"/>
     </row>
-    <row r="102" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -3592,7 +3593,7 @@
       <c r="AJ102" s="2"/>
       <c r="AK102" s="2"/>
     </row>
-    <row r="103" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="103" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
@@ -3619,7 +3620,7 @@
       <c r="AJ103" s="2"/>
       <c r="AK103" s="2"/>
     </row>
-    <row r="104" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="104" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M104" s="2"/>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -3646,7 +3647,7 @@
       <c r="AJ104" s="2"/>
       <c r="AK104" s="2"/>
     </row>
-    <row r="105" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="105" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
@@ -3673,7 +3674,7 @@
       <c r="AJ105" s="2"/>
       <c r="AK105" s="2"/>
     </row>
-    <row r="106" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="106" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
       <c r="O106" s="2"/>
@@ -3700,7 +3701,7 @@
       <c r="AJ106" s="2"/>
       <c r="AK106" s="2"/>
     </row>
-    <row r="107" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="107" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
@@ -3727,7 +3728,7 @@
       <c r="AJ107" s="2"/>
       <c r="AK107" s="2"/>
     </row>
-    <row r="108" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="108" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M108" s="2"/>
       <c r="N108" s="2"/>
       <c r="O108" s="2"/>
@@ -3754,7 +3755,7 @@
       <c r="AJ108" s="2"/>
       <c r="AK108" s="2"/>
     </row>
-    <row r="109" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="109" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M109" s="2"/>
       <c r="N109" s="2"/>
       <c r="O109" s="2"/>
@@ -3781,7 +3782,7 @@
       <c r="AJ109" s="2"/>
       <c r="AK109" s="2"/>
     </row>
-    <row r="110" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="110" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
       <c r="O110" s="2"/>
@@ -3808,7 +3809,7 @@
       <c r="AJ110" s="2"/>
       <c r="AK110" s="2"/>
     </row>
-    <row r="111" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="111" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
       <c r="O111" s="2"/>
@@ -3835,7 +3836,7 @@
       <c r="AJ111" s="2"/>
       <c r="AK111" s="2"/>
     </row>
-    <row r="112" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="112" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
       <c r="O112" s="2"/>
@@ -3862,7 +3863,7 @@
       <c r="AJ112" s="2"/>
       <c r="AK112" s="2"/>
     </row>
-    <row r="113" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
       <c r="O113" s="2"/>
@@ -3889,7 +3890,7 @@
       <c r="AJ113" s="2"/>
       <c r="AK113" s="2"/>
     </row>
-    <row r="114" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
       <c r="O114" s="2"/>
@@ -3916,7 +3917,7 @@
       <c r="AJ114" s="2"/>
       <c r="AK114" s="2"/>
     </row>
-    <row r="115" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
       <c r="O115" s="2"/>
@@ -3943,7 +3944,7 @@
       <c r="AJ115" s="2"/>
       <c r="AK115" s="2"/>
     </row>
-    <row r="116" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
       <c r="O116" s="2"/>
@@ -3970,7 +3971,7 @@
       <c r="AJ116" s="2"/>
       <c r="AK116" s="2"/>
     </row>
-    <row r="117" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="117" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
@@ -3997,7 +3998,7 @@
       <c r="AJ117" s="2"/>
       <c r="AK117" s="2"/>
     </row>
-    <row r="118" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="118" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
       <c r="O118" s="2"/>
@@ -4024,7 +4025,7 @@
       <c r="AJ118" s="2"/>
       <c r="AK118" s="2"/>
     </row>
-    <row r="119" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="119" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
       <c r="O119" s="2"/>
@@ -4051,7 +4052,7 @@
       <c r="AJ119" s="2"/>
       <c r="AK119" s="2"/>
     </row>
-    <row r="120" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="120" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M120" s="2"/>
       <c r="N120" s="2"/>
       <c r="O120" s="2"/>
@@ -4078,7 +4079,7 @@
       <c r="AJ120" s="2"/>
       <c r="AK120" s="2"/>
     </row>
-    <row r="121" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="121" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M121" s="2"/>
       <c r="N121" s="2"/>
       <c r="O121" s="2"/>
@@ -4105,7 +4106,7 @@
       <c r="AJ121" s="2"/>
       <c r="AK121" s="2"/>
     </row>
-    <row r="122" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="122" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
       <c r="O122" s="2"/>
@@ -4132,7 +4133,7 @@
       <c r="AJ122" s="2"/>
       <c r="AK122" s="2"/>
     </row>
-    <row r="123" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="123" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M123" s="2"/>
       <c r="N123" s="2"/>
       <c r="O123" s="2"/>
@@ -4159,7 +4160,7 @@
       <c r="AJ123" s="2"/>
       <c r="AK123" s="2"/>
     </row>
-    <row r="124" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="124" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M124" s="2"/>
       <c r="N124" s="2"/>
       <c r="O124" s="2"/>
@@ -4186,7 +4187,7 @@
       <c r="AJ124" s="2"/>
       <c r="AK124" s="2"/>
     </row>
-    <row r="125" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="125" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M125" s="2"/>
       <c r="N125" s="2"/>
       <c r="O125" s="2"/>
@@ -4213,7 +4214,7 @@
       <c r="AJ125" s="2"/>
       <c r="AK125" s="2"/>
     </row>
-    <row r="126" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="126" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
       <c r="O126" s="2"/>
@@ -4240,7 +4241,7 @@
       <c r="AJ126" s="2"/>
       <c r="AK126" s="2"/>
     </row>
-    <row r="127" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="127" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
       <c r="O127" s="2"/>
@@ -4267,7 +4268,7 @@
       <c r="AJ127" s="2"/>
       <c r="AK127" s="2"/>
     </row>
-    <row r="128" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="128" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M128" s="2"/>
       <c r="N128" s="2"/>
       <c r="O128" s="2"/>
@@ -4294,7 +4295,7 @@
       <c r="AJ128" s="2"/>
       <c r="AK128" s="2"/>
     </row>
-    <row r="129" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="129" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
       <c r="O129" s="2"/>
@@ -4321,7 +4322,7 @@
       <c r="AJ129" s="2"/>
       <c r="AK129" s="2"/>
     </row>
-    <row r="130" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="130" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M130" s="2"/>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
@@ -4348,7 +4349,7 @@
       <c r="AJ130" s="2"/>
       <c r="AK130" s="2"/>
     </row>
-    <row r="131" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="131" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M131" s="2"/>
       <c r="N131" s="2"/>
       <c r="O131" s="2"/>
@@ -4375,7 +4376,7 @@
       <c r="AJ131" s="2"/>
       <c r="AK131" s="2"/>
     </row>
-    <row r="132" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="132" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M132" s="2"/>
       <c r="N132" s="2"/>
       <c r="O132" s="2"/>
@@ -4402,7 +4403,7 @@
       <c r="AJ132" s="2"/>
       <c r="AK132" s="2"/>
     </row>
-    <row r="133" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="133" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M133" s="2"/>
       <c r="N133" s="2"/>
       <c r="O133" s="2"/>
@@ -4429,7 +4430,7 @@
       <c r="AJ133" s="2"/>
       <c r="AK133" s="2"/>
     </row>
-    <row r="134" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="134" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M134" s="2"/>
       <c r="N134" s="2"/>
       <c r="O134" s="2"/>
@@ -4456,7 +4457,7 @@
       <c r="AJ134" s="2"/>
       <c r="AK134" s="2"/>
     </row>
-    <row r="135" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="135" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M135" s="2"/>
       <c r="N135" s="2"/>
       <c r="O135" s="2"/>
@@ -4483,7 +4484,7 @@
       <c r="AJ135" s="2"/>
       <c r="AK135" s="2"/>
     </row>
-    <row r="136" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="136" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M136" s="2"/>
       <c r="N136" s="2"/>
       <c r="O136" s="2"/>
@@ -4510,7 +4511,7 @@
       <c r="AJ136" s="2"/>
       <c r="AK136" s="2"/>
     </row>
-    <row r="137" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="137" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M137" s="2"/>
       <c r="N137" s="2"/>
       <c r="O137" s="2"/>
@@ -4537,7 +4538,7 @@
       <c r="AJ137" s="2"/>
       <c r="AK137" s="2"/>
     </row>
-    <row r="138" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="138" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M138" s="2"/>
       <c r="N138" s="2"/>
       <c r="O138" s="2"/>
@@ -4564,7 +4565,7 @@
       <c r="AJ138" s="2"/>
       <c r="AK138" s="2"/>
     </row>
-    <row r="139" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="139" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M139" s="2"/>
       <c r="N139" s="2"/>
       <c r="O139" s="2"/>
@@ -4591,7 +4592,7 @@
       <c r="AJ139" s="2"/>
       <c r="AK139" s="2"/>
     </row>
-    <row r="140" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="140" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M140" s="2"/>
       <c r="N140" s="2"/>
       <c r="O140" s="2"/>
@@ -4618,7 +4619,7 @@
       <c r="AJ140" s="2"/>
       <c r="AK140" s="2"/>
     </row>
-    <row r="141" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="141" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M141" s="2"/>
       <c r="N141" s="2"/>
       <c r="O141" s="2"/>
@@ -4645,7 +4646,7 @@
       <c r="AJ141" s="2"/>
       <c r="AK141" s="2"/>
     </row>
-    <row r="142" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="142" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M142" s="2"/>
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
@@ -4672,7 +4673,7 @@
       <c r="AJ142" s="2"/>
       <c r="AK142" s="2"/>
     </row>
-    <row r="143" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="143" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M143" s="2"/>
       <c r="N143" s="2"/>
       <c r="O143" s="2"/>
@@ -4699,7 +4700,7 @@
       <c r="AJ143" s="2"/>
       <c r="AK143" s="2"/>
     </row>
-    <row r="144" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="144" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M144" s="2"/>
       <c r="N144" s="2"/>
       <c r="O144" s="2"/>
@@ -4726,7 +4727,7 @@
       <c r="AJ144" s="2"/>
       <c r="AK144" s="2"/>
     </row>
-    <row r="145" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="145" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M145" s="2"/>
       <c r="N145" s="2"/>
       <c r="O145" s="2"/>
@@ -4753,7 +4754,7 @@
       <c r="AJ145" s="2"/>
       <c r="AK145" s="2"/>
     </row>
-    <row r="146" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="146" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
@@ -4780,7 +4781,7 @@
       <c r="AJ146" s="2"/>
       <c r="AK146" s="2"/>
     </row>
-    <row r="147" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="147" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M147" s="2"/>
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
@@ -4807,7 +4808,7 @@
       <c r="AJ147" s="2"/>
       <c r="AK147" s="2"/>
     </row>
-    <row r="148" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="148" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
       <c r="O148" s="2"/>
@@ -4834,7 +4835,7 @@
       <c r="AJ148" s="2"/>
       <c r="AK148" s="2"/>
     </row>
-    <row r="149" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="149" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
@@ -4861,7 +4862,7 @@
       <c r="AJ149" s="2"/>
       <c r="AK149" s="2"/>
     </row>
-    <row r="150" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="150" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
       <c r="O150" s="2"/>
@@ -4888,7 +4889,7 @@
       <c r="AJ150" s="2"/>
       <c r="AK150" s="2"/>
     </row>
-    <row r="151" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="151" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M151" s="2"/>
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
@@ -4915,7 +4916,7 @@
       <c r="AJ151" s="2"/>
       <c r="AK151" s="2"/>
     </row>
-    <row r="152" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="152" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M152" s="2"/>
       <c r="N152" s="2"/>
       <c r="O152" s="2"/>
@@ -4942,7 +4943,7 @@
       <c r="AJ152" s="2"/>
       <c r="AK152" s="2"/>
     </row>
-    <row r="153" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="153" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M153" s="2"/>
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
@@ -4969,7 +4970,7 @@
       <c r="AJ153" s="2"/>
       <c r="AK153" s="2"/>
     </row>
-    <row r="154" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="154" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
       <c r="O154" s="2"/>
@@ -4996,7 +4997,7 @@
       <c r="AJ154" s="2"/>
       <c r="AK154" s="2"/>
     </row>
-    <row r="155" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="155" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M155" s="2"/>
       <c r="N155" s="2"/>
       <c r="O155" s="2"/>
@@ -5023,7 +5024,7 @@
       <c r="AJ155" s="2"/>
       <c r="AK155" s="2"/>
     </row>
-    <row r="156" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="156" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
       <c r="O156" s="2"/>
@@ -5050,7 +5051,7 @@
       <c r="AJ156" s="2"/>
       <c r="AK156" s="2"/>
     </row>
-    <row r="157" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="157" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
       <c r="O157" s="2"/>
@@ -5077,7 +5078,7 @@
       <c r="AJ157" s="2"/>
       <c r="AK157" s="2"/>
     </row>
-    <row r="158" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="158" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M158" s="2"/>
       <c r="N158" s="2"/>
       <c r="O158" s="2"/>
@@ -5104,7 +5105,7 @@
       <c r="AJ158" s="2"/>
       <c r="AK158" s="2"/>
     </row>
-    <row r="159" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="159" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M159" s="2"/>
       <c r="N159" s="2"/>
       <c r="O159" s="2"/>
@@ -5131,7 +5132,7 @@
       <c r="AJ159" s="2"/>
       <c r="AK159" s="2"/>
     </row>
-    <row r="160" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="160" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M160" s="2"/>
       <c r="N160" s="2"/>
       <c r="O160" s="2"/>
@@ -5158,7 +5159,7 @@
       <c r="AJ160" s="2"/>
       <c r="AK160" s="2"/>
     </row>
-    <row r="161" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="161" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
       <c r="O161" s="2"/>
@@ -5187,6 +5188,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A15:C18"/>
     <mergeCell ref="D15:F18"/>
     <mergeCell ref="G15:I18"/>
@@ -5200,13 +5208,6 @@
     <mergeCell ref="D11:F14"/>
     <mergeCell ref="G11:I14"/>
     <mergeCell ref="J11:L14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5214,21 +5215,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008EA8F6205B617B4CBD762DBD6D300502" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="000a41c94a85e4495c2f2d3453c30ed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10b95d85-a823-4616-89f6-0a6587d88b0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0729d4038857d2ede91d1e28869f4e90" ns3:_="">
     <xsd:import namespace="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
@@ -5374,10 +5360,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A39B317-7C09-4361-8F9C-EC6B55EB4D12}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5399,19 +5410,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A39B317-7C09-4361-8F9C-EC6B55EB4D12}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
patterns_element2 added and update on code_smells_element2
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nova pasta\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Faculdade\3º Ano\1º Semestre\ES\jabref\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA0F6A0-7CDF-4EF7-817F-72E509D5AA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDF6D35-2D44-4A24-9826-9FF50F7B5280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -70,11 +70,6 @@
     <t>Metrics</t>
   </si>
   <si>
-    <t>Member 2: detecting smells
-Member 1: detecting smells
-Member 5: detecting smells</t>
-  </si>
-  <si>
     <t>Member 5: finished code smells.
 Member 1: finished code smells.
 Member 2: finished code smells.</t>
@@ -87,6 +82,16 @@
   <si>
     <t xml:space="preserve">
 Member 1: Doing the metrics</t>
+  </si>
+  <si>
+    <t>Member 1: detecting smells
+Member 5: detecting smells</t>
+  </si>
+  <si>
+    <t>Member 1: gui package
+Member 3: model package
+Member 4: preferences package
+Member 5: cli package</t>
   </si>
 </sst>
 </file>
@@ -213,14 +218,29 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -232,21 +252,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -568,16 +573,16 @@
   <dimension ref="A1:AL161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="D3" sqref="D3:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -619,27 +624,27 @@
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
     </row>
-    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="14" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="14" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -666,27 +671,27 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
+      <c r="D3" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="6" t="s">
-        <v>10</v>
+      <c r="G3" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="9" t="s">
-        <v>11</v>
+      <c r="J3" s="14" t="s">
+        <v>10</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -713,19 +718,19 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -752,19 +757,19 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -791,19 +796,19 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -830,23 +835,23 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -873,19 +878,19 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -912,19 +917,19 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -951,19 +956,19 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -990,25 +995,25 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="13" t="s">
-        <v>12</v>
+      <c r="G11" s="12" t="s">
+        <v>11</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1035,19 +1040,19 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1074,19 +1079,19 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1113,19 +1118,19 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
+    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1152,25 +1157,25 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="13" t="s">
-        <v>13</v>
+      <c r="G15" s="12" t="s">
+        <v>12</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1197,19 +1202,19 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1236,19 +1241,19 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1275,19 +1280,19 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
-    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
+    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1314,7 +1319,7 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1341,7 +1346,7 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1368,7 +1373,7 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -1395,7 +1400,7 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -1422,7 +1427,7 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1449,7 +1454,7 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1476,7 +1481,7 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -1503,7 +1508,7 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -1530,7 +1535,7 @@
       <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1557,7 +1562,7 @@
       <c r="AJ27" s="2"/>
       <c r="AK27" s="2"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -1584,7 +1589,7 @@
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -1611,7 +1616,7 @@
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -1638,7 +1643,7 @@
       <c r="AJ30" s="2"/>
       <c r="AK30" s="2"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -1665,7 +1670,7 @@
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -1692,7 +1697,7 @@
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
     </row>
-    <row r="33" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -1719,7 +1724,7 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
     </row>
-    <row r="34" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -1746,7 +1751,7 @@
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
     </row>
-    <row r="35" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -1773,7 +1778,7 @@
       <c r="AJ35" s="2"/>
       <c r="AK35" s="2"/>
     </row>
-    <row r="36" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -1800,7 +1805,7 @@
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
     </row>
-    <row r="37" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -1827,7 +1832,7 @@
       <c r="AJ37" s="2"/>
       <c r="AK37" s="2"/>
     </row>
-    <row r="38" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -1854,7 +1859,7 @@
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
     </row>
-    <row r="39" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -1881,7 +1886,7 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
     </row>
-    <row r="40" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -1908,7 +1913,7 @@
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
     </row>
-    <row r="41" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -1935,7 +1940,7 @@
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
     </row>
-    <row r="42" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -1962,7 +1967,7 @@
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
     </row>
-    <row r="43" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -1989,7 +1994,7 @@
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
     </row>
-    <row r="44" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -2016,7 +2021,7 @@
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
     </row>
-    <row r="45" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -2043,7 +2048,7 @@
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
     </row>
-    <row r="46" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -2070,7 +2075,7 @@
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
     </row>
-    <row r="47" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -2097,7 +2102,7 @@
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
     </row>
-    <row r="48" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -2124,7 +2129,7 @@
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
     </row>
-    <row r="49" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -2151,7 +2156,7 @@
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2"/>
     </row>
-    <row r="50" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -2178,7 +2183,7 @@
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
     </row>
-    <row r="51" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -2205,7 +2210,7 @@
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
     </row>
-    <row r="52" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -2232,7 +2237,7 @@
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
     </row>
-    <row r="53" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -2259,7 +2264,7 @@
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
     </row>
-    <row r="54" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -2286,7 +2291,7 @@
       <c r="AJ54" s="2"/>
       <c r="AK54" s="2"/>
     </row>
-    <row r="55" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -2313,7 +2318,7 @@
       <c r="AJ55" s="2"/>
       <c r="AK55" s="2"/>
     </row>
-    <row r="56" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -2340,7 +2345,7 @@
       <c r="AJ56" s="2"/>
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -2367,7 +2372,7 @@
       <c r="AJ57" s="2"/>
       <c r="AK57" s="2"/>
     </row>
-    <row r="58" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -2394,7 +2399,7 @@
       <c r="AJ58" s="2"/>
       <c r="AK58" s="2"/>
     </row>
-    <row r="59" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -2421,7 +2426,7 @@
       <c r="AJ59" s="2"/>
       <c r="AK59" s="2"/>
     </row>
-    <row r="60" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="60" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -2448,7 +2453,7 @@
       <c r="AJ60" s="2"/>
       <c r="AK60" s="2"/>
     </row>
-    <row r="61" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -2475,7 +2480,7 @@
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
     </row>
-    <row r="62" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -2502,7 +2507,7 @@
       <c r="AJ62" s="2"/>
       <c r="AK62" s="2"/>
     </row>
-    <row r="63" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -2529,7 +2534,7 @@
       <c r="AJ63" s="2"/>
       <c r="AK63" s="2"/>
     </row>
-    <row r="64" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -2556,7 +2561,7 @@
       <c r="AJ64" s="2"/>
       <c r="AK64" s="2"/>
     </row>
-    <row r="65" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
@@ -2583,7 +2588,7 @@
       <c r="AJ65" s="2"/>
       <c r="AK65" s="2"/>
     </row>
-    <row r="66" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -2610,7 +2615,7 @@
       <c r="AJ66" s="2"/>
       <c r="AK66" s="2"/>
     </row>
-    <row r="67" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -2637,7 +2642,7 @@
       <c r="AJ67" s="2"/>
       <c r="AK67" s="2"/>
     </row>
-    <row r="68" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -2664,7 +2669,7 @@
       <c r="AJ68" s="2"/>
       <c r="AK68" s="2"/>
     </row>
-    <row r="69" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="69" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -2691,7 +2696,7 @@
       <c r="AJ69" s="2"/>
       <c r="AK69" s="2"/>
     </row>
-    <row r="70" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
@@ -2718,7 +2723,7 @@
       <c r="AJ70" s="2"/>
       <c r="AK70" s="2"/>
     </row>
-    <row r="71" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="71" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
@@ -2745,7 +2750,7 @@
       <c r="AJ71" s="2"/>
       <c r="AK71" s="2"/>
     </row>
-    <row r="72" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="72" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
@@ -2772,7 +2777,7 @@
       <c r="AJ72" s="2"/>
       <c r="AK72" s="2"/>
     </row>
-    <row r="73" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="73" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -2799,7 +2804,7 @@
       <c r="AJ73" s="2"/>
       <c r="AK73" s="2"/>
     </row>
-    <row r="74" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="74" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
@@ -2826,7 +2831,7 @@
       <c r="AJ74" s="2"/>
       <c r="AK74" s="2"/>
     </row>
-    <row r="75" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="75" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -2853,7 +2858,7 @@
       <c r="AJ75" s="2"/>
       <c r="AK75" s="2"/>
     </row>
-    <row r="76" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="76" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -2880,7 +2885,7 @@
       <c r="AJ76" s="2"/>
       <c r="AK76" s="2"/>
     </row>
-    <row r="77" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="77" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -2907,7 +2912,7 @@
       <c r="AJ77" s="2"/>
       <c r="AK77" s="2"/>
     </row>
-    <row r="78" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="78" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -2934,7 +2939,7 @@
       <c r="AJ78" s="2"/>
       <c r="AK78" s="2"/>
     </row>
-    <row r="79" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="79" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -2961,7 +2966,7 @@
       <c r="AJ79" s="2"/>
       <c r="AK79" s="2"/>
     </row>
-    <row r="80" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="80" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
@@ -2988,7 +2993,7 @@
       <c r="AJ80" s="2"/>
       <c r="AK80" s="2"/>
     </row>
-    <row r="81" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="81" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
@@ -3015,7 +3020,7 @@
       <c r="AJ81" s="2"/>
       <c r="AK81" s="2"/>
     </row>
-    <row r="82" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="82" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
@@ -3042,7 +3047,7 @@
       <c r="AJ82" s="2"/>
       <c r="AK82" s="2"/>
     </row>
-    <row r="83" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="83" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
@@ -3069,7 +3074,7 @@
       <c r="AJ83" s="2"/>
       <c r="AK83" s="2"/>
     </row>
-    <row r="84" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="84" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
@@ -3096,7 +3101,7 @@
       <c r="AJ84" s="2"/>
       <c r="AK84" s="2"/>
     </row>
-    <row r="85" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="85" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
@@ -3123,7 +3128,7 @@
       <c r="AJ85" s="2"/>
       <c r="AK85" s="2"/>
     </row>
-    <row r="86" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="86" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -3150,7 +3155,7 @@
       <c r="AJ86" s="2"/>
       <c r="AK86" s="2"/>
     </row>
-    <row r="87" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="87" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
@@ -3177,7 +3182,7 @@
       <c r="AJ87" s="2"/>
       <c r="AK87" s="2"/>
     </row>
-    <row r="88" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="88" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -3204,7 +3209,7 @@
       <c r="AJ88" s="2"/>
       <c r="AK88" s="2"/>
     </row>
-    <row r="89" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="89" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
@@ -3231,7 +3236,7 @@
       <c r="AJ89" s="2"/>
       <c r="AK89" s="2"/>
     </row>
-    <row r="90" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="90" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
@@ -3258,7 +3263,7 @@
       <c r="AJ90" s="2"/>
       <c r="AK90" s="2"/>
     </row>
-    <row r="91" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="91" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
@@ -3285,7 +3290,7 @@
       <c r="AJ91" s="2"/>
       <c r="AK91" s="2"/>
     </row>
-    <row r="92" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="92" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -3312,7 +3317,7 @@
       <c r="AJ92" s="2"/>
       <c r="AK92" s="2"/>
     </row>
-    <row r="93" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="93" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -3339,7 +3344,7 @@
       <c r="AJ93" s="2"/>
       <c r="AK93" s="2"/>
     </row>
-    <row r="94" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="94" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
@@ -3366,7 +3371,7 @@
       <c r="AJ94" s="2"/>
       <c r="AK94" s="2"/>
     </row>
-    <row r="95" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="95" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
@@ -3393,7 +3398,7 @@
       <c r="AJ95" s="2"/>
       <c r="AK95" s="2"/>
     </row>
-    <row r="96" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="96" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -3420,7 +3425,7 @@
       <c r="AJ96" s="2"/>
       <c r="AK96" s="2"/>
     </row>
-    <row r="97" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="97" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -3447,7 +3452,7 @@
       <c r="AJ97" s="2"/>
       <c r="AK97" s="2"/>
     </row>
-    <row r="98" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="98" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
@@ -3474,7 +3479,7 @@
       <c r="AJ98" s="2"/>
       <c r="AK98" s="2"/>
     </row>
-    <row r="99" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="99" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
@@ -3501,7 +3506,7 @@
       <c r="AJ99" s="2"/>
       <c r="AK99" s="2"/>
     </row>
-    <row r="100" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="100" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
@@ -3528,7 +3533,7 @@
       <c r="AJ100" s="2"/>
       <c r="AK100" s="2"/>
     </row>
-    <row r="101" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="101" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
@@ -3555,7 +3560,7 @@
       <c r="AJ101" s="2"/>
       <c r="AK101" s="2"/>
     </row>
-    <row r="102" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="102" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -3582,7 +3587,7 @@
       <c r="AJ102" s="2"/>
       <c r="AK102" s="2"/>
     </row>
-    <row r="103" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="103" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
@@ -3609,7 +3614,7 @@
       <c r="AJ103" s="2"/>
       <c r="AK103" s="2"/>
     </row>
-    <row r="104" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="104" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M104" s="2"/>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -3636,7 +3641,7 @@
       <c r="AJ104" s="2"/>
       <c r="AK104" s="2"/>
     </row>
-    <row r="105" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="105" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
@@ -3663,7 +3668,7 @@
       <c r="AJ105" s="2"/>
       <c r="AK105" s="2"/>
     </row>
-    <row r="106" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="106" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
       <c r="O106" s="2"/>
@@ -3690,7 +3695,7 @@
       <c r="AJ106" s="2"/>
       <c r="AK106" s="2"/>
     </row>
-    <row r="107" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="107" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
@@ -3717,7 +3722,7 @@
       <c r="AJ107" s="2"/>
       <c r="AK107" s="2"/>
     </row>
-    <row r="108" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="108" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M108" s="2"/>
       <c r="N108" s="2"/>
       <c r="O108" s="2"/>
@@ -3744,7 +3749,7 @@
       <c r="AJ108" s="2"/>
       <c r="AK108" s="2"/>
     </row>
-    <row r="109" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="109" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M109" s="2"/>
       <c r="N109" s="2"/>
       <c r="O109" s="2"/>
@@ -3771,7 +3776,7 @@
       <c r="AJ109" s="2"/>
       <c r="AK109" s="2"/>
     </row>
-    <row r="110" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="110" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
       <c r="O110" s="2"/>
@@ -3798,7 +3803,7 @@
       <c r="AJ110" s="2"/>
       <c r="AK110" s="2"/>
     </row>
-    <row r="111" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="111" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
       <c r="O111" s="2"/>
@@ -3825,7 +3830,7 @@
       <c r="AJ111" s="2"/>
       <c r="AK111" s="2"/>
     </row>
-    <row r="112" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="112" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
       <c r="O112" s="2"/>
@@ -3852,7 +3857,7 @@
       <c r="AJ112" s="2"/>
       <c r="AK112" s="2"/>
     </row>
-    <row r="113" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="113" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
       <c r="O113" s="2"/>
@@ -3879,7 +3884,7 @@
       <c r="AJ113" s="2"/>
       <c r="AK113" s="2"/>
     </row>
-    <row r="114" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="114" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
       <c r="O114" s="2"/>
@@ -3906,7 +3911,7 @@
       <c r="AJ114" s="2"/>
       <c r="AK114" s="2"/>
     </row>
-    <row r="115" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="115" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
       <c r="O115" s="2"/>
@@ -3933,7 +3938,7 @@
       <c r="AJ115" s="2"/>
       <c r="AK115" s="2"/>
     </row>
-    <row r="116" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="116" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
       <c r="O116" s="2"/>
@@ -3960,7 +3965,7 @@
       <c r="AJ116" s="2"/>
       <c r="AK116" s="2"/>
     </row>
-    <row r="117" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="117" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
@@ -3987,7 +3992,7 @@
       <c r="AJ117" s="2"/>
       <c r="AK117" s="2"/>
     </row>
-    <row r="118" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="118" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
       <c r="O118" s="2"/>
@@ -4014,7 +4019,7 @@
       <c r="AJ118" s="2"/>
       <c r="AK118" s="2"/>
     </row>
-    <row r="119" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="119" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
       <c r="O119" s="2"/>
@@ -4041,7 +4046,7 @@
       <c r="AJ119" s="2"/>
       <c r="AK119" s="2"/>
     </row>
-    <row r="120" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="120" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M120" s="2"/>
       <c r="N120" s="2"/>
       <c r="O120" s="2"/>
@@ -4068,7 +4073,7 @@
       <c r="AJ120" s="2"/>
       <c r="AK120" s="2"/>
     </row>
-    <row r="121" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="121" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M121" s="2"/>
       <c r="N121" s="2"/>
       <c r="O121" s="2"/>
@@ -4095,7 +4100,7 @@
       <c r="AJ121" s="2"/>
       <c r="AK121" s="2"/>
     </row>
-    <row r="122" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="122" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
       <c r="O122" s="2"/>
@@ -4122,7 +4127,7 @@
       <c r="AJ122" s="2"/>
       <c r="AK122" s="2"/>
     </row>
-    <row r="123" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="123" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M123" s="2"/>
       <c r="N123" s="2"/>
       <c r="O123" s="2"/>
@@ -4149,7 +4154,7 @@
       <c r="AJ123" s="2"/>
       <c r="AK123" s="2"/>
     </row>
-    <row r="124" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="124" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M124" s="2"/>
       <c r="N124" s="2"/>
       <c r="O124" s="2"/>
@@ -4176,7 +4181,7 @@
       <c r="AJ124" s="2"/>
       <c r="AK124" s="2"/>
     </row>
-    <row r="125" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="125" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M125" s="2"/>
       <c r="N125" s="2"/>
       <c r="O125" s="2"/>
@@ -4203,7 +4208,7 @@
       <c r="AJ125" s="2"/>
       <c r="AK125" s="2"/>
     </row>
-    <row r="126" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="126" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
       <c r="O126" s="2"/>
@@ -4230,7 +4235,7 @@
       <c r="AJ126" s="2"/>
       <c r="AK126" s="2"/>
     </row>
-    <row r="127" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="127" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
       <c r="O127" s="2"/>
@@ -4257,7 +4262,7 @@
       <c r="AJ127" s="2"/>
       <c r="AK127" s="2"/>
     </row>
-    <row r="128" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="128" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M128" s="2"/>
       <c r="N128" s="2"/>
       <c r="O128" s="2"/>
@@ -4284,7 +4289,7 @@
       <c r="AJ128" s="2"/>
       <c r="AK128" s="2"/>
     </row>
-    <row r="129" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="129" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
       <c r="O129" s="2"/>
@@ -4311,7 +4316,7 @@
       <c r="AJ129" s="2"/>
       <c r="AK129" s="2"/>
     </row>
-    <row r="130" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="130" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M130" s="2"/>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
@@ -4338,7 +4343,7 @@
       <c r="AJ130" s="2"/>
       <c r="AK130" s="2"/>
     </row>
-    <row r="131" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="131" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M131" s="2"/>
       <c r="N131" s="2"/>
       <c r="O131" s="2"/>
@@ -4365,7 +4370,7 @@
       <c r="AJ131" s="2"/>
       <c r="AK131" s="2"/>
     </row>
-    <row r="132" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="132" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M132" s="2"/>
       <c r="N132" s="2"/>
       <c r="O132" s="2"/>
@@ -4392,7 +4397,7 @@
       <c r="AJ132" s="2"/>
       <c r="AK132" s="2"/>
     </row>
-    <row r="133" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="133" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M133" s="2"/>
       <c r="N133" s="2"/>
       <c r="O133" s="2"/>
@@ -4419,7 +4424,7 @@
       <c r="AJ133" s="2"/>
       <c r="AK133" s="2"/>
     </row>
-    <row r="134" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="134" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M134" s="2"/>
       <c r="N134" s="2"/>
       <c r="O134" s="2"/>
@@ -4446,7 +4451,7 @@
       <c r="AJ134" s="2"/>
       <c r="AK134" s="2"/>
     </row>
-    <row r="135" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="135" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M135" s="2"/>
       <c r="N135" s="2"/>
       <c r="O135" s="2"/>
@@ -4473,7 +4478,7 @@
       <c r="AJ135" s="2"/>
       <c r="AK135" s="2"/>
     </row>
-    <row r="136" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="136" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M136" s="2"/>
       <c r="N136" s="2"/>
       <c r="O136" s="2"/>
@@ -4500,7 +4505,7 @@
       <c r="AJ136" s="2"/>
       <c r="AK136" s="2"/>
     </row>
-    <row r="137" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="137" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M137" s="2"/>
       <c r="N137" s="2"/>
       <c r="O137" s="2"/>
@@ -4527,7 +4532,7 @@
       <c r="AJ137" s="2"/>
       <c r="AK137" s="2"/>
     </row>
-    <row r="138" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="138" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M138" s="2"/>
       <c r="N138" s="2"/>
       <c r="O138" s="2"/>
@@ -4554,7 +4559,7 @@
       <c r="AJ138" s="2"/>
       <c r="AK138" s="2"/>
     </row>
-    <row r="139" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="139" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M139" s="2"/>
       <c r="N139" s="2"/>
       <c r="O139" s="2"/>
@@ -4581,7 +4586,7 @@
       <c r="AJ139" s="2"/>
       <c r="AK139" s="2"/>
     </row>
-    <row r="140" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="140" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M140" s="2"/>
       <c r="N140" s="2"/>
       <c r="O140" s="2"/>
@@ -4608,7 +4613,7 @@
       <c r="AJ140" s="2"/>
       <c r="AK140" s="2"/>
     </row>
-    <row r="141" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="141" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M141" s="2"/>
       <c r="N141" s="2"/>
       <c r="O141" s="2"/>
@@ -4635,7 +4640,7 @@
       <c r="AJ141" s="2"/>
       <c r="AK141" s="2"/>
     </row>
-    <row r="142" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="142" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M142" s="2"/>
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
@@ -4662,7 +4667,7 @@
       <c r="AJ142" s="2"/>
       <c r="AK142" s="2"/>
     </row>
-    <row r="143" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="143" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M143" s="2"/>
       <c r="N143" s="2"/>
       <c r="O143" s="2"/>
@@ -4689,7 +4694,7 @@
       <c r="AJ143" s="2"/>
       <c r="AK143" s="2"/>
     </row>
-    <row r="144" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="144" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M144" s="2"/>
       <c r="N144" s="2"/>
       <c r="O144" s="2"/>
@@ -4716,7 +4721,7 @@
       <c r="AJ144" s="2"/>
       <c r="AK144" s="2"/>
     </row>
-    <row r="145" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="145" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M145" s="2"/>
       <c r="N145" s="2"/>
       <c r="O145" s="2"/>
@@ -4743,7 +4748,7 @@
       <c r="AJ145" s="2"/>
       <c r="AK145" s="2"/>
     </row>
-    <row r="146" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="146" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
@@ -4770,7 +4775,7 @@
       <c r="AJ146" s="2"/>
       <c r="AK146" s="2"/>
     </row>
-    <row r="147" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="147" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M147" s="2"/>
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
@@ -4797,7 +4802,7 @@
       <c r="AJ147" s="2"/>
       <c r="AK147" s="2"/>
     </row>
-    <row r="148" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="148" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
       <c r="O148" s="2"/>
@@ -4824,7 +4829,7 @@
       <c r="AJ148" s="2"/>
       <c r="AK148" s="2"/>
     </row>
-    <row r="149" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="149" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
@@ -4851,7 +4856,7 @@
       <c r="AJ149" s="2"/>
       <c r="AK149" s="2"/>
     </row>
-    <row r="150" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="150" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
       <c r="O150" s="2"/>
@@ -4878,7 +4883,7 @@
       <c r="AJ150" s="2"/>
       <c r="AK150" s="2"/>
     </row>
-    <row r="151" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="151" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M151" s="2"/>
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
@@ -4905,7 +4910,7 @@
       <c r="AJ151" s="2"/>
       <c r="AK151" s="2"/>
     </row>
-    <row r="152" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="152" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M152" s="2"/>
       <c r="N152" s="2"/>
       <c r="O152" s="2"/>
@@ -4932,7 +4937,7 @@
       <c r="AJ152" s="2"/>
       <c r="AK152" s="2"/>
     </row>
-    <row r="153" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="153" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M153" s="2"/>
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
@@ -4959,7 +4964,7 @@
       <c r="AJ153" s="2"/>
       <c r="AK153" s="2"/>
     </row>
-    <row r="154" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="154" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
       <c r="O154" s="2"/>
@@ -4986,7 +4991,7 @@
       <c r="AJ154" s="2"/>
       <c r="AK154" s="2"/>
     </row>
-    <row r="155" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="155" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M155" s="2"/>
       <c r="N155" s="2"/>
       <c r="O155" s="2"/>
@@ -5013,7 +5018,7 @@
       <c r="AJ155" s="2"/>
       <c r="AK155" s="2"/>
     </row>
-    <row r="156" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="156" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
       <c r="O156" s="2"/>
@@ -5040,7 +5045,7 @@
       <c r="AJ156" s="2"/>
       <c r="AK156" s="2"/>
     </row>
-    <row r="157" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="157" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
       <c r="O157" s="2"/>
@@ -5067,7 +5072,7 @@
       <c r="AJ157" s="2"/>
       <c r="AK157" s="2"/>
     </row>
-    <row r="158" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="158" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M158" s="2"/>
       <c r="N158" s="2"/>
       <c r="O158" s="2"/>
@@ -5094,7 +5099,7 @@
       <c r="AJ158" s="2"/>
       <c r="AK158" s="2"/>
     </row>
-    <row r="159" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="159" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M159" s="2"/>
       <c r="N159" s="2"/>
       <c r="O159" s="2"/>
@@ -5121,7 +5126,7 @@
       <c r="AJ159" s="2"/>
       <c r="AK159" s="2"/>
     </row>
-    <row r="160" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="160" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M160" s="2"/>
       <c r="N160" s="2"/>
       <c r="O160" s="2"/>
@@ -5148,7 +5153,7 @@
       <c r="AJ160" s="2"/>
       <c r="AK160" s="2"/>
     </row>
-    <row r="161" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="161" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
       <c r="O161" s="2"/>
@@ -5177,13 +5182,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A15:C18"/>
     <mergeCell ref="D15:F18"/>
     <mergeCell ref="G15:I18"/>
@@ -5197,6 +5195,13 @@
     <mergeCell ref="D11:F14"/>
     <mergeCell ref="G11:I14"/>
     <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5204,18 +5209,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5365,6 +5370,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5376,14 +5389,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
elem2 sprint backlog update
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Faculdade\3º Ano\1º Semestre\ES\jabref\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDF6D35-2D44-4A24-9826-9FF50F7B5280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7D3474-DA51-465E-918B-0AF5F980119E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -92,6 +92,9 @@
 Member 3: model package
 Member 4: preferences package
 Member 5: cli package</t>
+  </si>
+  <si>
+    <t>Member 2: making diagrams</t>
   </si>
 </sst>
 </file>
@@ -218,25 +221,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -252,6 +243,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -573,16 +576,16 @@
   <dimension ref="A1:AL161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F6"/>
+      <selection activeCell="J11" sqref="J11:L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="46.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -624,27 +627,27 @@
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
     </row>
-    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -671,27 +674,27 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -718,19 +721,19 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -757,19 +760,19 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -796,19 +799,19 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
+    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -835,23 +838,25 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
+      <c r="G7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -878,19 +883,19 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -917,19 +922,19 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -956,19 +961,19 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -995,25 +1000,25 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="10" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1040,19 +1045,19 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1079,19 +1084,19 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1118,19 +1123,19 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
+    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1157,25 +1162,25 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1202,19 +1207,19 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1241,19 +1246,19 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1280,19 +1285,19 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
-    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
+    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1319,7 +1324,7 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1346,7 +1351,7 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1373,7 +1378,7 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -1400,7 +1405,7 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -1427,7 +1432,7 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1454,7 +1459,7 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1481,7 +1486,7 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -1508,7 +1513,7 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -1535,7 +1540,7 @@
       <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1562,7 +1567,7 @@
       <c r="AJ27" s="2"/>
       <c r="AK27" s="2"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -1589,7 +1594,7 @@
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -1616,7 +1621,7 @@
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -1643,7 +1648,7 @@
       <c r="AJ30" s="2"/>
       <c r="AK30" s="2"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -1670,7 +1675,7 @@
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -1697,7 +1702,7 @@
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
     </row>
-    <row r="33" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -1724,7 +1729,7 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
     </row>
-    <row r="34" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -1751,7 +1756,7 @@
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
     </row>
-    <row r="35" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -1778,7 +1783,7 @@
       <c r="AJ35" s="2"/>
       <c r="AK35" s="2"/>
     </row>
-    <row r="36" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -1805,7 +1810,7 @@
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
     </row>
-    <row r="37" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -1832,7 +1837,7 @@
       <c r="AJ37" s="2"/>
       <c r="AK37" s="2"/>
     </row>
-    <row r="38" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -1859,7 +1864,7 @@
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
     </row>
-    <row r="39" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -1886,7 +1891,7 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
     </row>
-    <row r="40" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -1913,7 +1918,7 @@
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
     </row>
-    <row r="41" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -1940,7 +1945,7 @@
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
     </row>
-    <row r="42" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -1967,7 +1972,7 @@
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
     </row>
-    <row r="43" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -1994,7 +1999,7 @@
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
     </row>
-    <row r="44" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -2021,7 +2026,7 @@
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
     </row>
-    <row r="45" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -2048,7 +2053,7 @@
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
     </row>
-    <row r="46" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -2075,7 +2080,7 @@
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
     </row>
-    <row r="47" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -2102,7 +2107,7 @@
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
     </row>
-    <row r="48" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -2129,7 +2134,7 @@
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
     </row>
-    <row r="49" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -2156,7 +2161,7 @@
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2"/>
     </row>
-    <row r="50" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -2183,7 +2188,7 @@
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
     </row>
-    <row r="51" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -2210,7 +2215,7 @@
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
     </row>
-    <row r="52" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -2237,7 +2242,7 @@
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
     </row>
-    <row r="53" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -2264,7 +2269,7 @@
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
     </row>
-    <row r="54" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -2291,7 +2296,7 @@
       <c r="AJ54" s="2"/>
       <c r="AK54" s="2"/>
     </row>
-    <row r="55" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -2318,7 +2323,7 @@
       <c r="AJ55" s="2"/>
       <c r="AK55" s="2"/>
     </row>
-    <row r="56" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -2345,7 +2350,7 @@
       <c r="AJ56" s="2"/>
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -2372,7 +2377,7 @@
       <c r="AJ57" s="2"/>
       <c r="AK57" s="2"/>
     </row>
-    <row r="58" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -2399,7 +2404,7 @@
       <c r="AJ58" s="2"/>
       <c r="AK58" s="2"/>
     </row>
-    <row r="59" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -2426,7 +2431,7 @@
       <c r="AJ59" s="2"/>
       <c r="AK59" s="2"/>
     </row>
-    <row r="60" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -2453,7 +2458,7 @@
       <c r="AJ60" s="2"/>
       <c r="AK60" s="2"/>
     </row>
-    <row r="61" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -2480,7 +2485,7 @@
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
     </row>
-    <row r="62" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -2507,7 +2512,7 @@
       <c r="AJ62" s="2"/>
       <c r="AK62" s="2"/>
     </row>
-    <row r="63" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -2534,7 +2539,7 @@
       <c r="AJ63" s="2"/>
       <c r="AK63" s="2"/>
     </row>
-    <row r="64" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -2561,7 +2566,7 @@
       <c r="AJ64" s="2"/>
       <c r="AK64" s="2"/>
     </row>
-    <row r="65" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
@@ -2588,7 +2593,7 @@
       <c r="AJ65" s="2"/>
       <c r="AK65" s="2"/>
     </row>
-    <row r="66" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -2615,7 +2620,7 @@
       <c r="AJ66" s="2"/>
       <c r="AK66" s="2"/>
     </row>
-    <row r="67" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -2642,7 +2647,7 @@
       <c r="AJ67" s="2"/>
       <c r="AK67" s="2"/>
     </row>
-    <row r="68" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -2669,7 +2674,7 @@
       <c r="AJ68" s="2"/>
       <c r="AK68" s="2"/>
     </row>
-    <row r="69" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -2696,7 +2701,7 @@
       <c r="AJ69" s="2"/>
       <c r="AK69" s="2"/>
     </row>
-    <row r="70" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
@@ -2723,7 +2728,7 @@
       <c r="AJ70" s="2"/>
       <c r="AK70" s="2"/>
     </row>
-    <row r="71" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
@@ -2750,7 +2755,7 @@
       <c r="AJ71" s="2"/>
       <c r="AK71" s="2"/>
     </row>
-    <row r="72" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
@@ -2777,7 +2782,7 @@
       <c r="AJ72" s="2"/>
       <c r="AK72" s="2"/>
     </row>
-    <row r="73" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -2804,7 +2809,7 @@
       <c r="AJ73" s="2"/>
       <c r="AK73" s="2"/>
     </row>
-    <row r="74" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
@@ -2831,7 +2836,7 @@
       <c r="AJ74" s="2"/>
       <c r="AK74" s="2"/>
     </row>
-    <row r="75" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="75" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -2858,7 +2863,7 @@
       <c r="AJ75" s="2"/>
       <c r="AK75" s="2"/>
     </row>
-    <row r="76" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="76" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -2885,7 +2890,7 @@
       <c r="AJ76" s="2"/>
       <c r="AK76" s="2"/>
     </row>
-    <row r="77" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="77" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -2912,7 +2917,7 @@
       <c r="AJ77" s="2"/>
       <c r="AK77" s="2"/>
     </row>
-    <row r="78" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="78" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -2939,7 +2944,7 @@
       <c r="AJ78" s="2"/>
       <c r="AK78" s="2"/>
     </row>
-    <row r="79" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="79" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -2966,7 +2971,7 @@
       <c r="AJ79" s="2"/>
       <c r="AK79" s="2"/>
     </row>
-    <row r="80" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="80" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
@@ -2993,7 +2998,7 @@
       <c r="AJ80" s="2"/>
       <c r="AK80" s="2"/>
     </row>
-    <row r="81" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="81" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
@@ -3020,7 +3025,7 @@
       <c r="AJ81" s="2"/>
       <c r="AK81" s="2"/>
     </row>
-    <row r="82" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="82" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
@@ -3047,7 +3052,7 @@
       <c r="AJ82" s="2"/>
       <c r="AK82" s="2"/>
     </row>
-    <row r="83" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="83" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
@@ -3074,7 +3079,7 @@
       <c r="AJ83" s="2"/>
       <c r="AK83" s="2"/>
     </row>
-    <row r="84" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="84" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
@@ -3101,7 +3106,7 @@
       <c r="AJ84" s="2"/>
       <c r="AK84" s="2"/>
     </row>
-    <row r="85" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="85" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
@@ -3128,7 +3133,7 @@
       <c r="AJ85" s="2"/>
       <c r="AK85" s="2"/>
     </row>
-    <row r="86" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="86" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -3155,7 +3160,7 @@
       <c r="AJ86" s="2"/>
       <c r="AK86" s="2"/>
     </row>
-    <row r="87" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="87" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
@@ -3182,7 +3187,7 @@
       <c r="AJ87" s="2"/>
       <c r="AK87" s="2"/>
     </row>
-    <row r="88" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="88" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -3209,7 +3214,7 @@
       <c r="AJ88" s="2"/>
       <c r="AK88" s="2"/>
     </row>
-    <row r="89" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="89" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
@@ -3236,7 +3241,7 @@
       <c r="AJ89" s="2"/>
       <c r="AK89" s="2"/>
     </row>
-    <row r="90" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="90" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
@@ -3263,7 +3268,7 @@
       <c r="AJ90" s="2"/>
       <c r="AK90" s="2"/>
     </row>
-    <row r="91" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="91" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
@@ -3290,7 +3295,7 @@
       <c r="AJ91" s="2"/>
       <c r="AK91" s="2"/>
     </row>
-    <row r="92" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="92" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -3317,7 +3322,7 @@
       <c r="AJ92" s="2"/>
       <c r="AK92" s="2"/>
     </row>
-    <row r="93" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="93" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -3344,7 +3349,7 @@
       <c r="AJ93" s="2"/>
       <c r="AK93" s="2"/>
     </row>
-    <row r="94" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="94" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
@@ -3371,7 +3376,7 @@
       <c r="AJ94" s="2"/>
       <c r="AK94" s="2"/>
     </row>
-    <row r="95" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="95" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
@@ -3398,7 +3403,7 @@
       <c r="AJ95" s="2"/>
       <c r="AK95" s="2"/>
     </row>
-    <row r="96" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="96" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -3425,7 +3430,7 @@
       <c r="AJ96" s="2"/>
       <c r="AK96" s="2"/>
     </row>
-    <row r="97" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="97" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -3452,7 +3457,7 @@
       <c r="AJ97" s="2"/>
       <c r="AK97" s="2"/>
     </row>
-    <row r="98" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
@@ -3479,7 +3484,7 @@
       <c r="AJ98" s="2"/>
       <c r="AK98" s="2"/>
     </row>
-    <row r="99" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="99" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
@@ -3506,7 +3511,7 @@
       <c r="AJ99" s="2"/>
       <c r="AK99" s="2"/>
     </row>
-    <row r="100" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="100" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
@@ -3533,7 +3538,7 @@
       <c r="AJ100" s="2"/>
       <c r="AK100" s="2"/>
     </row>
-    <row r="101" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="101" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
@@ -3560,7 +3565,7 @@
       <c r="AJ101" s="2"/>
       <c r="AK101" s="2"/>
     </row>
-    <row r="102" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -3587,7 +3592,7 @@
       <c r="AJ102" s="2"/>
       <c r="AK102" s="2"/>
     </row>
-    <row r="103" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="103" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
@@ -3614,7 +3619,7 @@
       <c r="AJ103" s="2"/>
       <c r="AK103" s="2"/>
     </row>
-    <row r="104" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="104" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M104" s="2"/>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -3641,7 +3646,7 @@
       <c r="AJ104" s="2"/>
       <c r="AK104" s="2"/>
     </row>
-    <row r="105" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="105" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
@@ -3668,7 +3673,7 @@
       <c r="AJ105" s="2"/>
       <c r="AK105" s="2"/>
     </row>
-    <row r="106" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="106" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
       <c r="O106" s="2"/>
@@ -3695,7 +3700,7 @@
       <c r="AJ106" s="2"/>
       <c r="AK106" s="2"/>
     </row>
-    <row r="107" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="107" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
@@ -3722,7 +3727,7 @@
       <c r="AJ107" s="2"/>
       <c r="AK107" s="2"/>
     </row>
-    <row r="108" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="108" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M108" s="2"/>
       <c r="N108" s="2"/>
       <c r="O108" s="2"/>
@@ -3749,7 +3754,7 @@
       <c r="AJ108" s="2"/>
       <c r="AK108" s="2"/>
     </row>
-    <row r="109" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="109" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M109" s="2"/>
       <c r="N109" s="2"/>
       <c r="O109" s="2"/>
@@ -3776,7 +3781,7 @@
       <c r="AJ109" s="2"/>
       <c r="AK109" s="2"/>
     </row>
-    <row r="110" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="110" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
       <c r="O110" s="2"/>
@@ -3803,7 +3808,7 @@
       <c r="AJ110" s="2"/>
       <c r="AK110" s="2"/>
     </row>
-    <row r="111" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="111" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
       <c r="O111" s="2"/>
@@ -3830,7 +3835,7 @@
       <c r="AJ111" s="2"/>
       <c r="AK111" s="2"/>
     </row>
-    <row r="112" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="112" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
       <c r="O112" s="2"/>
@@ -3857,7 +3862,7 @@
       <c r="AJ112" s="2"/>
       <c r="AK112" s="2"/>
     </row>
-    <row r="113" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
       <c r="O113" s="2"/>
@@ -3884,7 +3889,7 @@
       <c r="AJ113" s="2"/>
       <c r="AK113" s="2"/>
     </row>
-    <row r="114" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
       <c r="O114" s="2"/>
@@ -3911,7 +3916,7 @@
       <c r="AJ114" s="2"/>
       <c r="AK114" s="2"/>
     </row>
-    <row r="115" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
       <c r="O115" s="2"/>
@@ -3938,7 +3943,7 @@
       <c r="AJ115" s="2"/>
       <c r="AK115" s="2"/>
     </row>
-    <row r="116" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
       <c r="O116" s="2"/>
@@ -3965,7 +3970,7 @@
       <c r="AJ116" s="2"/>
       <c r="AK116" s="2"/>
     </row>
-    <row r="117" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="117" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
@@ -3992,7 +3997,7 @@
       <c r="AJ117" s="2"/>
       <c r="AK117" s="2"/>
     </row>
-    <row r="118" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="118" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
       <c r="O118" s="2"/>
@@ -4019,7 +4024,7 @@
       <c r="AJ118" s="2"/>
       <c r="AK118" s="2"/>
     </row>
-    <row r="119" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="119" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
       <c r="O119" s="2"/>
@@ -4046,7 +4051,7 @@
       <c r="AJ119" s="2"/>
       <c r="AK119" s="2"/>
     </row>
-    <row r="120" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="120" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M120" s="2"/>
       <c r="N120" s="2"/>
       <c r="O120" s="2"/>
@@ -4073,7 +4078,7 @@
       <c r="AJ120" s="2"/>
       <c r="AK120" s="2"/>
     </row>
-    <row r="121" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="121" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M121" s="2"/>
       <c r="N121" s="2"/>
       <c r="O121" s="2"/>
@@ -4100,7 +4105,7 @@
       <c r="AJ121" s="2"/>
       <c r="AK121" s="2"/>
     </row>
-    <row r="122" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="122" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
       <c r="O122" s="2"/>
@@ -4127,7 +4132,7 @@
       <c r="AJ122" s="2"/>
       <c r="AK122" s="2"/>
     </row>
-    <row r="123" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="123" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M123" s="2"/>
       <c r="N123" s="2"/>
       <c r="O123" s="2"/>
@@ -4154,7 +4159,7 @@
       <c r="AJ123" s="2"/>
       <c r="AK123" s="2"/>
     </row>
-    <row r="124" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="124" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M124" s="2"/>
       <c r="N124" s="2"/>
       <c r="O124" s="2"/>
@@ -4181,7 +4186,7 @@
       <c r="AJ124" s="2"/>
       <c r="AK124" s="2"/>
     </row>
-    <row r="125" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="125" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M125" s="2"/>
       <c r="N125" s="2"/>
       <c r="O125" s="2"/>
@@ -4208,7 +4213,7 @@
       <c r="AJ125" s="2"/>
       <c r="AK125" s="2"/>
     </row>
-    <row r="126" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="126" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
       <c r="O126" s="2"/>
@@ -4235,7 +4240,7 @@
       <c r="AJ126" s="2"/>
       <c r="AK126" s="2"/>
     </row>
-    <row r="127" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="127" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
       <c r="O127" s="2"/>
@@ -4262,7 +4267,7 @@
       <c r="AJ127" s="2"/>
       <c r="AK127" s="2"/>
     </row>
-    <row r="128" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="128" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M128" s="2"/>
       <c r="N128" s="2"/>
       <c r="O128" s="2"/>
@@ -4289,7 +4294,7 @@
       <c r="AJ128" s="2"/>
       <c r="AK128" s="2"/>
     </row>
-    <row r="129" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="129" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
       <c r="O129" s="2"/>
@@ -4316,7 +4321,7 @@
       <c r="AJ129" s="2"/>
       <c r="AK129" s="2"/>
     </row>
-    <row r="130" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="130" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M130" s="2"/>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
@@ -4343,7 +4348,7 @@
       <c r="AJ130" s="2"/>
       <c r="AK130" s="2"/>
     </row>
-    <row r="131" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="131" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M131" s="2"/>
       <c r="N131" s="2"/>
       <c r="O131" s="2"/>
@@ -4370,7 +4375,7 @@
       <c r="AJ131" s="2"/>
       <c r="AK131" s="2"/>
     </row>
-    <row r="132" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="132" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M132" s="2"/>
       <c r="N132" s="2"/>
       <c r="O132" s="2"/>
@@ -4397,7 +4402,7 @@
       <c r="AJ132" s="2"/>
       <c r="AK132" s="2"/>
     </row>
-    <row r="133" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="133" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M133" s="2"/>
       <c r="N133" s="2"/>
       <c r="O133" s="2"/>
@@ -4424,7 +4429,7 @@
       <c r="AJ133" s="2"/>
       <c r="AK133" s="2"/>
     </row>
-    <row r="134" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="134" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M134" s="2"/>
       <c r="N134" s="2"/>
       <c r="O134" s="2"/>
@@ -4451,7 +4456,7 @@
       <c r="AJ134" s="2"/>
       <c r="AK134" s="2"/>
     </row>
-    <row r="135" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="135" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M135" s="2"/>
       <c r="N135" s="2"/>
       <c r="O135" s="2"/>
@@ -4478,7 +4483,7 @@
       <c r="AJ135" s="2"/>
       <c r="AK135" s="2"/>
     </row>
-    <row r="136" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="136" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M136" s="2"/>
       <c r="N136" s="2"/>
       <c r="O136" s="2"/>
@@ -4505,7 +4510,7 @@
       <c r="AJ136" s="2"/>
       <c r="AK136" s="2"/>
     </row>
-    <row r="137" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="137" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M137" s="2"/>
       <c r="N137" s="2"/>
       <c r="O137" s="2"/>
@@ -4532,7 +4537,7 @@
       <c r="AJ137" s="2"/>
       <c r="AK137" s="2"/>
     </row>
-    <row r="138" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="138" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M138" s="2"/>
       <c r="N138" s="2"/>
       <c r="O138" s="2"/>
@@ -4559,7 +4564,7 @@
       <c r="AJ138" s="2"/>
       <c r="AK138" s="2"/>
     </row>
-    <row r="139" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="139" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M139" s="2"/>
       <c r="N139" s="2"/>
       <c r="O139" s="2"/>
@@ -4586,7 +4591,7 @@
       <c r="AJ139" s="2"/>
       <c r="AK139" s="2"/>
     </row>
-    <row r="140" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="140" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M140" s="2"/>
       <c r="N140" s="2"/>
       <c r="O140" s="2"/>
@@ -4613,7 +4618,7 @@
       <c r="AJ140" s="2"/>
       <c r="AK140" s="2"/>
     </row>
-    <row r="141" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="141" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M141" s="2"/>
       <c r="N141" s="2"/>
       <c r="O141" s="2"/>
@@ -4640,7 +4645,7 @@
       <c r="AJ141" s="2"/>
       <c r="AK141" s="2"/>
     </row>
-    <row r="142" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="142" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M142" s="2"/>
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
@@ -4667,7 +4672,7 @@
       <c r="AJ142" s="2"/>
       <c r="AK142" s="2"/>
     </row>
-    <row r="143" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="143" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M143" s="2"/>
       <c r="N143" s="2"/>
       <c r="O143" s="2"/>
@@ -4694,7 +4699,7 @@
       <c r="AJ143" s="2"/>
       <c r="AK143" s="2"/>
     </row>
-    <row r="144" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="144" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M144" s="2"/>
       <c r="N144" s="2"/>
       <c r="O144" s="2"/>
@@ -4721,7 +4726,7 @@
       <c r="AJ144" s="2"/>
       <c r="AK144" s="2"/>
     </row>
-    <row r="145" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="145" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M145" s="2"/>
       <c r="N145" s="2"/>
       <c r="O145" s="2"/>
@@ -4748,7 +4753,7 @@
       <c r="AJ145" s="2"/>
       <c r="AK145" s="2"/>
     </row>
-    <row r="146" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="146" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
@@ -4775,7 +4780,7 @@
       <c r="AJ146" s="2"/>
       <c r="AK146" s="2"/>
     </row>
-    <row r="147" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="147" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M147" s="2"/>
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
@@ -4802,7 +4807,7 @@
       <c r="AJ147" s="2"/>
       <c r="AK147" s="2"/>
     </row>
-    <row r="148" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="148" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
       <c r="O148" s="2"/>
@@ -4829,7 +4834,7 @@
       <c r="AJ148" s="2"/>
       <c r="AK148" s="2"/>
     </row>
-    <row r="149" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="149" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
@@ -4856,7 +4861,7 @@
       <c r="AJ149" s="2"/>
       <c r="AK149" s="2"/>
     </row>
-    <row r="150" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="150" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
       <c r="O150" s="2"/>
@@ -4883,7 +4888,7 @@
       <c r="AJ150" s="2"/>
       <c r="AK150" s="2"/>
     </row>
-    <row r="151" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="151" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M151" s="2"/>
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
@@ -4910,7 +4915,7 @@
       <c r="AJ151" s="2"/>
       <c r="AK151" s="2"/>
     </row>
-    <row r="152" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="152" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M152" s="2"/>
       <c r="N152" s="2"/>
       <c r="O152" s="2"/>
@@ -4937,7 +4942,7 @@
       <c r="AJ152" s="2"/>
       <c r="AK152" s="2"/>
     </row>
-    <row r="153" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="153" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M153" s="2"/>
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
@@ -4964,7 +4969,7 @@
       <c r="AJ153" s="2"/>
       <c r="AK153" s="2"/>
     </row>
-    <row r="154" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="154" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
       <c r="O154" s="2"/>
@@ -4991,7 +4996,7 @@
       <c r="AJ154" s="2"/>
       <c r="AK154" s="2"/>
     </row>
-    <row r="155" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="155" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M155" s="2"/>
       <c r="N155" s="2"/>
       <c r="O155" s="2"/>
@@ -5018,7 +5023,7 @@
       <c r="AJ155" s="2"/>
       <c r="AK155" s="2"/>
     </row>
-    <row r="156" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="156" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
       <c r="O156" s="2"/>
@@ -5045,7 +5050,7 @@
       <c r="AJ156" s="2"/>
       <c r="AK156" s="2"/>
     </row>
-    <row r="157" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="157" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
       <c r="O157" s="2"/>
@@ -5072,7 +5077,7 @@
       <c r="AJ157" s="2"/>
       <c r="AK157" s="2"/>
     </row>
-    <row r="158" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="158" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M158" s="2"/>
       <c r="N158" s="2"/>
       <c r="O158" s="2"/>
@@ -5099,7 +5104,7 @@
       <c r="AJ158" s="2"/>
       <c r="AK158" s="2"/>
     </row>
-    <row r="159" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="159" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M159" s="2"/>
       <c r="N159" s="2"/>
       <c r="O159" s="2"/>
@@ -5126,7 +5131,7 @@
       <c r="AJ159" s="2"/>
       <c r="AK159" s="2"/>
     </row>
-    <row r="160" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="160" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M160" s="2"/>
       <c r="N160" s="2"/>
       <c r="O160" s="2"/>
@@ -5153,7 +5158,7 @@
       <c r="AJ160" s="2"/>
       <c r="AK160" s="2"/>
     </row>
-    <row r="161" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="161" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
       <c r="O161" s="2"/>
@@ -5182,6 +5187,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A15:C18"/>
     <mergeCell ref="D15:F18"/>
     <mergeCell ref="G15:I18"/>
@@ -5195,13 +5207,6 @@
     <mergeCell ref="D11:F14"/>
     <mergeCell ref="G11:I14"/>
     <mergeCell ref="J11:L14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5209,18 +5214,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5370,14 +5375,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5389,6 +5386,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
patterns_element2 done and elem2 sprint backlog update
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Faculdade\3º Ano\1º Semestre\ES\jabref\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7D3474-DA51-465E-918B-0AF5F980119E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF2F7C2-2D22-4532-AD90-19212AD14974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -75,11 +75,6 @@
 Member 2: finished code smells.</t>
   </si>
   <si>
-    <t>Member 5: detecting patterns.
-Member 2: detecting patterns.
-Member 1: detecting patterns.</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Member 1: Doing the metrics</t>
   </si>
@@ -95,6 +90,13 @@
   </si>
   <si>
     <t>Member 2: making diagrams</t>
+  </si>
+  <si>
+    <t>Member 2: finished pattern detection</t>
+  </si>
+  <si>
+    <t>Member 5: detecting patterns.
+Member 1: detecting patterns.</t>
   </si>
 </sst>
 </file>
@@ -221,13 +223,25 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -243,18 +257,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -575,17 +577,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0899AEA-CFD5-4FE7-96CD-5876EC28C07C}">
   <dimension ref="A1:AL161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:L14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15:L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -627,27 +629,27 @@
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
     </row>
-    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="14" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="14" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -674,27 +676,27 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
+      <c r="D3" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="6" t="s">
-        <v>13</v>
+      <c r="G3" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -721,19 +723,19 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -760,19 +762,19 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -799,19 +801,19 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -838,25 +840,25 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="5" t="s">
-        <v>15</v>
+      <c r="G7" s="11" t="s">
+        <v>14</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -883,19 +885,19 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -922,19 +924,19 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -961,19 +963,19 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1000,25 +1002,27 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="8" t="s">
-        <v>11</v>
+      <c r="G11" s="12" t="s">
+        <v>16</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1045,19 +1049,19 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1084,19 +1088,19 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1123,19 +1127,19 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
+    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1162,25 +1166,25 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="8" t="s">
-        <v>12</v>
+      <c r="G15" s="12" t="s">
+        <v>11</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1207,19 +1211,19 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1246,19 +1250,19 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1285,19 +1289,19 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
-    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1324,7 +1328,7 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1351,7 +1355,7 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1378,7 +1382,7 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -1405,7 +1409,7 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -1432,7 +1436,7 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1459,7 +1463,7 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1486,7 +1490,7 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -1513,7 +1517,7 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -1540,7 +1544,7 @@
       <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1567,7 +1571,7 @@
       <c r="AJ27" s="2"/>
       <c r="AK27" s="2"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -1594,7 +1598,7 @@
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -1621,7 +1625,7 @@
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -1648,7 +1652,7 @@
       <c r="AJ30" s="2"/>
       <c r="AK30" s="2"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -1675,7 +1679,7 @@
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -1702,7 +1706,7 @@
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
     </row>
-    <row r="33" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -1729,7 +1733,7 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
     </row>
-    <row r="34" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -1756,7 +1760,7 @@
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
     </row>
-    <row r="35" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -1783,7 +1787,7 @@
       <c r="AJ35" s="2"/>
       <c r="AK35" s="2"/>
     </row>
-    <row r="36" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -1810,7 +1814,7 @@
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
     </row>
-    <row r="37" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -1837,7 +1841,7 @@
       <c r="AJ37" s="2"/>
       <c r="AK37" s="2"/>
     </row>
-    <row r="38" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -1864,7 +1868,7 @@
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
     </row>
-    <row r="39" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -1891,7 +1895,7 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
     </row>
-    <row r="40" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -1918,7 +1922,7 @@
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
     </row>
-    <row r="41" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -1945,7 +1949,7 @@
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
     </row>
-    <row r="42" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -1972,7 +1976,7 @@
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
     </row>
-    <row r="43" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -1999,7 +2003,7 @@
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
     </row>
-    <row r="44" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -2026,7 +2030,7 @@
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
     </row>
-    <row r="45" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -2053,7 +2057,7 @@
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
     </row>
-    <row r="46" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -2080,7 +2084,7 @@
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
     </row>
-    <row r="47" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -2107,7 +2111,7 @@
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
     </row>
-    <row r="48" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -2134,7 +2138,7 @@
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
     </row>
-    <row r="49" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -2161,7 +2165,7 @@
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2"/>
     </row>
-    <row r="50" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -2188,7 +2192,7 @@
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
     </row>
-    <row r="51" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -2215,7 +2219,7 @@
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
     </row>
-    <row r="52" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -2242,7 +2246,7 @@
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
     </row>
-    <row r="53" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -2269,7 +2273,7 @@
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
     </row>
-    <row r="54" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -2296,7 +2300,7 @@
       <c r="AJ54" s="2"/>
       <c r="AK54" s="2"/>
     </row>
-    <row r="55" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -2323,7 +2327,7 @@
       <c r="AJ55" s="2"/>
       <c r="AK55" s="2"/>
     </row>
-    <row r="56" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -2350,7 +2354,7 @@
       <c r="AJ56" s="2"/>
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -2377,7 +2381,7 @@
       <c r="AJ57" s="2"/>
       <c r="AK57" s="2"/>
     </row>
-    <row r="58" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -2404,7 +2408,7 @@
       <c r="AJ58" s="2"/>
       <c r="AK58" s="2"/>
     </row>
-    <row r="59" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -2431,7 +2435,7 @@
       <c r="AJ59" s="2"/>
       <c r="AK59" s="2"/>
     </row>
-    <row r="60" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="60" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -2458,7 +2462,7 @@
       <c r="AJ60" s="2"/>
       <c r="AK60" s="2"/>
     </row>
-    <row r="61" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -2485,7 +2489,7 @@
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
     </row>
-    <row r="62" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -2512,7 +2516,7 @@
       <c r="AJ62" s="2"/>
       <c r="AK62" s="2"/>
     </row>
-    <row r="63" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -2539,7 +2543,7 @@
       <c r="AJ63" s="2"/>
       <c r="AK63" s="2"/>
     </row>
-    <row r="64" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -2566,7 +2570,7 @@
       <c r="AJ64" s="2"/>
       <c r="AK64" s="2"/>
     </row>
-    <row r="65" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
@@ -2593,7 +2597,7 @@
       <c r="AJ65" s="2"/>
       <c r="AK65" s="2"/>
     </row>
-    <row r="66" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -2620,7 +2624,7 @@
       <c r="AJ66" s="2"/>
       <c r="AK66" s="2"/>
     </row>
-    <row r="67" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -2647,7 +2651,7 @@
       <c r="AJ67" s="2"/>
       <c r="AK67" s="2"/>
     </row>
-    <row r="68" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -2674,7 +2678,7 @@
       <c r="AJ68" s="2"/>
       <c r="AK68" s="2"/>
     </row>
-    <row r="69" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="69" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -2701,7 +2705,7 @@
       <c r="AJ69" s="2"/>
       <c r="AK69" s="2"/>
     </row>
-    <row r="70" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
@@ -2728,7 +2732,7 @@
       <c r="AJ70" s="2"/>
       <c r="AK70" s="2"/>
     </row>
-    <row r="71" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="71" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
@@ -2755,7 +2759,7 @@
       <c r="AJ71" s="2"/>
       <c r="AK71" s="2"/>
     </row>
-    <row r="72" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="72" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
@@ -2782,7 +2786,7 @@
       <c r="AJ72" s="2"/>
       <c r="AK72" s="2"/>
     </row>
-    <row r="73" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="73" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -2809,7 +2813,7 @@
       <c r="AJ73" s="2"/>
       <c r="AK73" s="2"/>
     </row>
-    <row r="74" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="74" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
@@ -2836,7 +2840,7 @@
       <c r="AJ74" s="2"/>
       <c r="AK74" s="2"/>
     </row>
-    <row r="75" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="75" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -2863,7 +2867,7 @@
       <c r="AJ75" s="2"/>
       <c r="AK75" s="2"/>
     </row>
-    <row r="76" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="76" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -2890,7 +2894,7 @@
       <c r="AJ76" s="2"/>
       <c r="AK76" s="2"/>
     </row>
-    <row r="77" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="77" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -2917,7 +2921,7 @@
       <c r="AJ77" s="2"/>
       <c r="AK77" s="2"/>
     </row>
-    <row r="78" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="78" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -2944,7 +2948,7 @@
       <c r="AJ78" s="2"/>
       <c r="AK78" s="2"/>
     </row>
-    <row r="79" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="79" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -2971,7 +2975,7 @@
       <c r="AJ79" s="2"/>
       <c r="AK79" s="2"/>
     </row>
-    <row r="80" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="80" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
@@ -2998,7 +3002,7 @@
       <c r="AJ80" s="2"/>
       <c r="AK80" s="2"/>
     </row>
-    <row r="81" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="81" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
@@ -3025,7 +3029,7 @@
       <c r="AJ81" s="2"/>
       <c r="AK81" s="2"/>
     </row>
-    <row r="82" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="82" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
@@ -3052,7 +3056,7 @@
       <c r="AJ82" s="2"/>
       <c r="AK82" s="2"/>
     </row>
-    <row r="83" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="83" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
@@ -3079,7 +3083,7 @@
       <c r="AJ83" s="2"/>
       <c r="AK83" s="2"/>
     </row>
-    <row r="84" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="84" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
@@ -3106,7 +3110,7 @@
       <c r="AJ84" s="2"/>
       <c r="AK84" s="2"/>
     </row>
-    <row r="85" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="85" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
@@ -3133,7 +3137,7 @@
       <c r="AJ85" s="2"/>
       <c r="AK85" s="2"/>
     </row>
-    <row r="86" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="86" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -3160,7 +3164,7 @@
       <c r="AJ86" s="2"/>
       <c r="AK86" s="2"/>
     </row>
-    <row r="87" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="87" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
@@ -3187,7 +3191,7 @@
       <c r="AJ87" s="2"/>
       <c r="AK87" s="2"/>
     </row>
-    <row r="88" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="88" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -3214,7 +3218,7 @@
       <c r="AJ88" s="2"/>
       <c r="AK88" s="2"/>
     </row>
-    <row r="89" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="89" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
@@ -3241,7 +3245,7 @@
       <c r="AJ89" s="2"/>
       <c r="AK89" s="2"/>
     </row>
-    <row r="90" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="90" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
@@ -3268,7 +3272,7 @@
       <c r="AJ90" s="2"/>
       <c r="AK90" s="2"/>
     </row>
-    <row r="91" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="91" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
@@ -3295,7 +3299,7 @@
       <c r="AJ91" s="2"/>
       <c r="AK91" s="2"/>
     </row>
-    <row r="92" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="92" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -3322,7 +3326,7 @@
       <c r="AJ92" s="2"/>
       <c r="AK92" s="2"/>
     </row>
-    <row r="93" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="93" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -3349,7 +3353,7 @@
       <c r="AJ93" s="2"/>
       <c r="AK93" s="2"/>
     </row>
-    <row r="94" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="94" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
@@ -3376,7 +3380,7 @@
       <c r="AJ94" s="2"/>
       <c r="AK94" s="2"/>
     </row>
-    <row r="95" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="95" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
@@ -3403,7 +3407,7 @@
       <c r="AJ95" s="2"/>
       <c r="AK95" s="2"/>
     </row>
-    <row r="96" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="96" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -3430,7 +3434,7 @@
       <c r="AJ96" s="2"/>
       <c r="AK96" s="2"/>
     </row>
-    <row r="97" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="97" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -3457,7 +3461,7 @@
       <c r="AJ97" s="2"/>
       <c r="AK97" s="2"/>
     </row>
-    <row r="98" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="98" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
@@ -3484,7 +3488,7 @@
       <c r="AJ98" s="2"/>
       <c r="AK98" s="2"/>
     </row>
-    <row r="99" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="99" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
@@ -3511,7 +3515,7 @@
       <c r="AJ99" s="2"/>
       <c r="AK99" s="2"/>
     </row>
-    <row r="100" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="100" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
@@ -3538,7 +3542,7 @@
       <c r="AJ100" s="2"/>
       <c r="AK100" s="2"/>
     </row>
-    <row r="101" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="101" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
@@ -3565,7 +3569,7 @@
       <c r="AJ101" s="2"/>
       <c r="AK101" s="2"/>
     </row>
-    <row r="102" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="102" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -3592,7 +3596,7 @@
       <c r="AJ102" s="2"/>
       <c r="AK102" s="2"/>
     </row>
-    <row r="103" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="103" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
@@ -3619,7 +3623,7 @@
       <c r="AJ103" s="2"/>
       <c r="AK103" s="2"/>
     </row>
-    <row r="104" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="104" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M104" s="2"/>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -3646,7 +3650,7 @@
       <c r="AJ104" s="2"/>
       <c r="AK104" s="2"/>
     </row>
-    <row r="105" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="105" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
@@ -3673,7 +3677,7 @@
       <c r="AJ105" s="2"/>
       <c r="AK105" s="2"/>
     </row>
-    <row r="106" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="106" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
       <c r="O106" s="2"/>
@@ -3700,7 +3704,7 @@
       <c r="AJ106" s="2"/>
       <c r="AK106" s="2"/>
     </row>
-    <row r="107" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="107" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
@@ -3727,7 +3731,7 @@
       <c r="AJ107" s="2"/>
       <c r="AK107" s="2"/>
     </row>
-    <row r="108" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="108" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M108" s="2"/>
       <c r="N108" s="2"/>
       <c r="O108" s="2"/>
@@ -3754,7 +3758,7 @@
       <c r="AJ108" s="2"/>
       <c r="AK108" s="2"/>
     </row>
-    <row r="109" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="109" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M109" s="2"/>
       <c r="N109" s="2"/>
       <c r="O109" s="2"/>
@@ -3781,7 +3785,7 @@
       <c r="AJ109" s="2"/>
       <c r="AK109" s="2"/>
     </row>
-    <row r="110" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="110" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
       <c r="O110" s="2"/>
@@ -3808,7 +3812,7 @@
       <c r="AJ110" s="2"/>
       <c r="AK110" s="2"/>
     </row>
-    <row r="111" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="111" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
       <c r="O111" s="2"/>
@@ -3835,7 +3839,7 @@
       <c r="AJ111" s="2"/>
       <c r="AK111" s="2"/>
     </row>
-    <row r="112" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="112" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
       <c r="O112" s="2"/>
@@ -3862,7 +3866,7 @@
       <c r="AJ112" s="2"/>
       <c r="AK112" s="2"/>
     </row>
-    <row r="113" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="113" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
       <c r="O113" s="2"/>
@@ -3889,7 +3893,7 @@
       <c r="AJ113" s="2"/>
       <c r="AK113" s="2"/>
     </row>
-    <row r="114" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="114" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
       <c r="O114" s="2"/>
@@ -3916,7 +3920,7 @@
       <c r="AJ114" s="2"/>
       <c r="AK114" s="2"/>
     </row>
-    <row r="115" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="115" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
       <c r="O115" s="2"/>
@@ -3943,7 +3947,7 @@
       <c r="AJ115" s="2"/>
       <c r="AK115" s="2"/>
     </row>
-    <row r="116" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="116" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
       <c r="O116" s="2"/>
@@ -3970,7 +3974,7 @@
       <c r="AJ116" s="2"/>
       <c r="AK116" s="2"/>
     </row>
-    <row r="117" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="117" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
@@ -3997,7 +4001,7 @@
       <c r="AJ117" s="2"/>
       <c r="AK117" s="2"/>
     </row>
-    <row r="118" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="118" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
       <c r="O118" s="2"/>
@@ -4024,7 +4028,7 @@
       <c r="AJ118" s="2"/>
       <c r="AK118" s="2"/>
     </row>
-    <row r="119" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="119" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
       <c r="O119" s="2"/>
@@ -4051,7 +4055,7 @@
       <c r="AJ119" s="2"/>
       <c r="AK119" s="2"/>
     </row>
-    <row r="120" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="120" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M120" s="2"/>
       <c r="N120" s="2"/>
       <c r="O120" s="2"/>
@@ -4078,7 +4082,7 @@
       <c r="AJ120" s="2"/>
       <c r="AK120" s="2"/>
     </row>
-    <row r="121" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="121" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M121" s="2"/>
       <c r="N121" s="2"/>
       <c r="O121" s="2"/>
@@ -4105,7 +4109,7 @@
       <c r="AJ121" s="2"/>
       <c r="AK121" s="2"/>
     </row>
-    <row r="122" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="122" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
       <c r="O122" s="2"/>
@@ -4132,7 +4136,7 @@
       <c r="AJ122" s="2"/>
       <c r="AK122" s="2"/>
     </row>
-    <row r="123" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="123" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M123" s="2"/>
       <c r="N123" s="2"/>
       <c r="O123" s="2"/>
@@ -4159,7 +4163,7 @@
       <c r="AJ123" s="2"/>
       <c r="AK123" s="2"/>
     </row>
-    <row r="124" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="124" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M124" s="2"/>
       <c r="N124" s="2"/>
       <c r="O124" s="2"/>
@@ -4186,7 +4190,7 @@
       <c r="AJ124" s="2"/>
       <c r="AK124" s="2"/>
     </row>
-    <row r="125" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="125" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M125" s="2"/>
       <c r="N125" s="2"/>
       <c r="O125" s="2"/>
@@ -4213,7 +4217,7 @@
       <c r="AJ125" s="2"/>
       <c r="AK125" s="2"/>
     </row>
-    <row r="126" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="126" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
       <c r="O126" s="2"/>
@@ -4240,7 +4244,7 @@
       <c r="AJ126" s="2"/>
       <c r="AK126" s="2"/>
     </row>
-    <row r="127" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="127" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
       <c r="O127" s="2"/>
@@ -4267,7 +4271,7 @@
       <c r="AJ127" s="2"/>
       <c r="AK127" s="2"/>
     </row>
-    <row r="128" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="128" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M128" s="2"/>
       <c r="N128" s="2"/>
       <c r="O128" s="2"/>
@@ -4294,7 +4298,7 @@
       <c r="AJ128" s="2"/>
       <c r="AK128" s="2"/>
     </row>
-    <row r="129" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="129" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
       <c r="O129" s="2"/>
@@ -4321,7 +4325,7 @@
       <c r="AJ129" s="2"/>
       <c r="AK129" s="2"/>
     </row>
-    <row r="130" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="130" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M130" s="2"/>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
@@ -4348,7 +4352,7 @@
       <c r="AJ130" s="2"/>
       <c r="AK130" s="2"/>
     </row>
-    <row r="131" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="131" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M131" s="2"/>
       <c r="N131" s="2"/>
       <c r="O131" s="2"/>
@@ -4375,7 +4379,7 @@
       <c r="AJ131" s="2"/>
       <c r="AK131" s="2"/>
     </row>
-    <row r="132" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="132" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M132" s="2"/>
       <c r="N132" s="2"/>
       <c r="O132" s="2"/>
@@ -4402,7 +4406,7 @@
       <c r="AJ132" s="2"/>
       <c r="AK132" s="2"/>
     </row>
-    <row r="133" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="133" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M133" s="2"/>
       <c r="N133" s="2"/>
       <c r="O133" s="2"/>
@@ -4429,7 +4433,7 @@
       <c r="AJ133" s="2"/>
       <c r="AK133" s="2"/>
     </row>
-    <row r="134" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="134" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M134" s="2"/>
       <c r="N134" s="2"/>
       <c r="O134" s="2"/>
@@ -4456,7 +4460,7 @@
       <c r="AJ134" s="2"/>
       <c r="AK134" s="2"/>
     </row>
-    <row r="135" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="135" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M135" s="2"/>
       <c r="N135" s="2"/>
       <c r="O135" s="2"/>
@@ -4483,7 +4487,7 @@
       <c r="AJ135" s="2"/>
       <c r="AK135" s="2"/>
     </row>
-    <row r="136" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="136" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M136" s="2"/>
       <c r="N136" s="2"/>
       <c r="O136" s="2"/>
@@ -4510,7 +4514,7 @@
       <c r="AJ136" s="2"/>
       <c r="AK136" s="2"/>
     </row>
-    <row r="137" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="137" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M137" s="2"/>
       <c r="N137" s="2"/>
       <c r="O137" s="2"/>
@@ -4537,7 +4541,7 @@
       <c r="AJ137" s="2"/>
       <c r="AK137" s="2"/>
     </row>
-    <row r="138" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="138" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M138" s="2"/>
       <c r="N138" s="2"/>
       <c r="O138" s="2"/>
@@ -4564,7 +4568,7 @@
       <c r="AJ138" s="2"/>
       <c r="AK138" s="2"/>
     </row>
-    <row r="139" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="139" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M139" s="2"/>
       <c r="N139" s="2"/>
       <c r="O139" s="2"/>
@@ -4591,7 +4595,7 @@
       <c r="AJ139" s="2"/>
       <c r="AK139" s="2"/>
     </row>
-    <row r="140" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="140" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M140" s="2"/>
       <c r="N140" s="2"/>
       <c r="O140" s="2"/>
@@ -4618,7 +4622,7 @@
       <c r="AJ140" s="2"/>
       <c r="AK140" s="2"/>
     </row>
-    <row r="141" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="141" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M141" s="2"/>
       <c r="N141" s="2"/>
       <c r="O141" s="2"/>
@@ -4645,7 +4649,7 @@
       <c r="AJ141" s="2"/>
       <c r="AK141" s="2"/>
     </row>
-    <row r="142" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="142" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M142" s="2"/>
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
@@ -4672,7 +4676,7 @@
       <c r="AJ142" s="2"/>
       <c r="AK142" s="2"/>
     </row>
-    <row r="143" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="143" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M143" s="2"/>
       <c r="N143" s="2"/>
       <c r="O143" s="2"/>
@@ -4699,7 +4703,7 @@
       <c r="AJ143" s="2"/>
       <c r="AK143" s="2"/>
     </row>
-    <row r="144" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="144" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M144" s="2"/>
       <c r="N144" s="2"/>
       <c r="O144" s="2"/>
@@ -4726,7 +4730,7 @@
       <c r="AJ144" s="2"/>
       <c r="AK144" s="2"/>
     </row>
-    <row r="145" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="145" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M145" s="2"/>
       <c r="N145" s="2"/>
       <c r="O145" s="2"/>
@@ -4753,7 +4757,7 @@
       <c r="AJ145" s="2"/>
       <c r="AK145" s="2"/>
     </row>
-    <row r="146" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="146" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
@@ -4780,7 +4784,7 @@
       <c r="AJ146" s="2"/>
       <c r="AK146" s="2"/>
     </row>
-    <row r="147" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="147" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M147" s="2"/>
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
@@ -4807,7 +4811,7 @@
       <c r="AJ147" s="2"/>
       <c r="AK147" s="2"/>
     </row>
-    <row r="148" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="148" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
       <c r="O148" s="2"/>
@@ -4834,7 +4838,7 @@
       <c r="AJ148" s="2"/>
       <c r="AK148" s="2"/>
     </row>
-    <row r="149" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="149" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
@@ -4861,7 +4865,7 @@
       <c r="AJ149" s="2"/>
       <c r="AK149" s="2"/>
     </row>
-    <row r="150" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="150" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
       <c r="O150" s="2"/>
@@ -4888,7 +4892,7 @@
       <c r="AJ150" s="2"/>
       <c r="AK150" s="2"/>
     </row>
-    <row r="151" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="151" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M151" s="2"/>
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
@@ -4915,7 +4919,7 @@
       <c r="AJ151" s="2"/>
       <c r="AK151" s="2"/>
     </row>
-    <row r="152" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="152" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M152" s="2"/>
       <c r="N152" s="2"/>
       <c r="O152" s="2"/>
@@ -4942,7 +4946,7 @@
       <c r="AJ152" s="2"/>
       <c r="AK152" s="2"/>
     </row>
-    <row r="153" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="153" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M153" s="2"/>
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
@@ -4969,7 +4973,7 @@
       <c r="AJ153" s="2"/>
       <c r="AK153" s="2"/>
     </row>
-    <row r="154" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="154" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
       <c r="O154" s="2"/>
@@ -4996,7 +5000,7 @@
       <c r="AJ154" s="2"/>
       <c r="AK154" s="2"/>
     </row>
-    <row r="155" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="155" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M155" s="2"/>
       <c r="N155" s="2"/>
       <c r="O155" s="2"/>
@@ -5023,7 +5027,7 @@
       <c r="AJ155" s="2"/>
       <c r="AK155" s="2"/>
     </row>
-    <row r="156" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="156" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
       <c r="O156" s="2"/>
@@ -5050,7 +5054,7 @@
       <c r="AJ156" s="2"/>
       <c r="AK156" s="2"/>
     </row>
-    <row r="157" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="157" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
       <c r="O157" s="2"/>
@@ -5077,7 +5081,7 @@
       <c r="AJ157" s="2"/>
       <c r="AK157" s="2"/>
     </row>
-    <row r="158" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="158" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M158" s="2"/>
       <c r="N158" s="2"/>
       <c r="O158" s="2"/>
@@ -5104,7 +5108,7 @@
       <c r="AJ158" s="2"/>
       <c r="AK158" s="2"/>
     </row>
-    <row r="159" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="159" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M159" s="2"/>
       <c r="N159" s="2"/>
       <c r="O159" s="2"/>
@@ -5131,7 +5135,7 @@
       <c r="AJ159" s="2"/>
       <c r="AK159" s="2"/>
     </row>
-    <row r="160" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="160" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M160" s="2"/>
       <c r="N160" s="2"/>
       <c r="O160" s="2"/>
@@ -5158,7 +5162,7 @@
       <c r="AJ160" s="2"/>
       <c r="AK160" s="2"/>
     </row>
-    <row r="161" spans="13:37" x14ac:dyDescent="0.25">
+    <row r="161" spans="13:37" x14ac:dyDescent="0.3">
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
       <c r="O161" s="2"/>
@@ -5187,13 +5191,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A15:C18"/>
     <mergeCell ref="D15:F18"/>
     <mergeCell ref="G15:I18"/>
@@ -5207,6 +5204,13 @@
     <mergeCell ref="D11:F14"/>
     <mergeCell ref="G11:I14"/>
     <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5214,18 +5218,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5375,6 +5379,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5386,14 +5398,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
code smells member 2 update; data collected metrics member 2 incomplete and sprint backlog update
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Faculdade\3º Ano\1º Semestre\ES\jabref\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D26193E-C452-4050-BC2C-AC8B12630608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37974987-E365-41E5-8DBA-AA79F515EE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -75,10 +75,6 @@
 Member 2: finished code smells.</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Member 1: Doing the metrics</t>
-  </si>
-  <si>
     <t>Member 1: gui package
 Member 3: model package
 Member 4: preferences package</t>
@@ -105,6 +101,11 @@
   <si>
     <t>Member 2: finished pattern detection
 Member 5: finished pattern detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Member 1: Doing the metrics
+Member 2: Doing the metrics</t>
   </si>
 </sst>
 </file>
@@ -231,20 +232,29 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -255,17 +265,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -586,16 +587,16 @@
   <dimension ref="A1:AL161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:L18"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="46.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -637,27 +638,27 @@
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
     </row>
-    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="14" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="14" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -684,27 +685,27 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="6" t="s">
-        <v>12</v>
+      <c r="D3" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="6" t="s">
-        <v>13</v>
+      <c r="G3" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -731,19 +732,19 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -770,19 +771,19 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -809,19 +810,19 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -848,25 +849,25 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="8" t="s">
-        <v>17</v>
+      <c r="G7" s="12" t="s">
+        <v>16</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -893,19 +894,19 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -932,19 +933,19 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -971,19 +972,19 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1010,27 +1011,27 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6" t="s">
-        <v>14</v>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="8" t="s">
-        <v>15</v>
+      <c r="G11" s="12" t="s">
+        <v>14</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="8" t="s">
-        <v>18</v>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12" t="s">
+        <v>17</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1057,19 +1058,19 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1096,19 +1097,19 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1135,19 +1136,19 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1174,27 +1175,27 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6" t="s">
-        <v>14</v>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="8" t="s">
-        <v>11</v>
+      <c r="G15" s="12" t="s">
+        <v>18</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5" t="s">
-        <v>16</v>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11" t="s">
+        <v>15</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1221,19 +1222,19 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1260,19 +1261,19 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1299,19 +1300,19 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
-    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1338,7 +1339,7 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1365,7 +1366,7 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1392,7 +1393,7 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -1419,7 +1420,7 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -1446,7 +1447,7 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1473,7 +1474,7 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1500,7 +1501,7 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -1527,7 +1528,7 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -1554,7 +1555,7 @@
       <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1581,7 +1582,7 @@
       <c r="AJ27" s="2"/>
       <c r="AK27" s="2"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -1608,7 +1609,7 @@
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -1635,7 +1636,7 @@
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -1662,7 +1663,7 @@
       <c r="AJ30" s="2"/>
       <c r="AK30" s="2"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -1689,7 +1690,7 @@
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -1716,7 +1717,7 @@
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
     </row>
-    <row r="33" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -1743,7 +1744,7 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
     </row>
-    <row r="34" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -1770,7 +1771,7 @@
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
     </row>
-    <row r="35" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -1797,7 +1798,7 @@
       <c r="AJ35" s="2"/>
       <c r="AK35" s="2"/>
     </row>
-    <row r="36" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -1824,7 +1825,7 @@
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
     </row>
-    <row r="37" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -1851,7 +1852,7 @@
       <c r="AJ37" s="2"/>
       <c r="AK37" s="2"/>
     </row>
-    <row r="38" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -1878,7 +1879,7 @@
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
     </row>
-    <row r="39" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -1905,7 +1906,7 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
     </row>
-    <row r="40" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -1932,7 +1933,7 @@
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
     </row>
-    <row r="41" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -1959,7 +1960,7 @@
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
     </row>
-    <row r="42" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -1986,7 +1987,7 @@
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
     </row>
-    <row r="43" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -2013,7 +2014,7 @@
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
     </row>
-    <row r="44" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -2040,7 +2041,7 @@
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
     </row>
-    <row r="45" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -2067,7 +2068,7 @@
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
     </row>
-    <row r="46" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -2094,7 +2095,7 @@
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
     </row>
-    <row r="47" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -2121,7 +2122,7 @@
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
     </row>
-    <row r="48" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -2148,7 +2149,7 @@
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
     </row>
-    <row r="49" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -2175,7 +2176,7 @@
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2"/>
     </row>
-    <row r="50" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -2202,7 +2203,7 @@
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
     </row>
-    <row r="51" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -2229,7 +2230,7 @@
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
     </row>
-    <row r="52" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -2256,7 +2257,7 @@
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
     </row>
-    <row r="53" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -2283,7 +2284,7 @@
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
     </row>
-    <row r="54" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -2310,7 +2311,7 @@
       <c r="AJ54" s="2"/>
       <c r="AK54" s="2"/>
     </row>
-    <row r="55" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -2337,7 +2338,7 @@
       <c r="AJ55" s="2"/>
       <c r="AK55" s="2"/>
     </row>
-    <row r="56" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -2364,7 +2365,7 @@
       <c r="AJ56" s="2"/>
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -2391,7 +2392,7 @@
       <c r="AJ57" s="2"/>
       <c r="AK57" s="2"/>
     </row>
-    <row r="58" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -2418,7 +2419,7 @@
       <c r="AJ58" s="2"/>
       <c r="AK58" s="2"/>
     </row>
-    <row r="59" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -2445,7 +2446,7 @@
       <c r="AJ59" s="2"/>
       <c r="AK59" s="2"/>
     </row>
-    <row r="60" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -2472,7 +2473,7 @@
       <c r="AJ60" s="2"/>
       <c r="AK60" s="2"/>
     </row>
-    <row r="61" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -2499,7 +2500,7 @@
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
     </row>
-    <row r="62" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -2526,7 +2527,7 @@
       <c r="AJ62" s="2"/>
       <c r="AK62" s="2"/>
     </row>
-    <row r="63" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -2553,7 +2554,7 @@
       <c r="AJ63" s="2"/>
       <c r="AK63" s="2"/>
     </row>
-    <row r="64" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -2580,7 +2581,7 @@
       <c r="AJ64" s="2"/>
       <c r="AK64" s="2"/>
     </row>
-    <row r="65" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
@@ -2607,7 +2608,7 @@
       <c r="AJ65" s="2"/>
       <c r="AK65" s="2"/>
     </row>
-    <row r="66" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -2634,7 +2635,7 @@
       <c r="AJ66" s="2"/>
       <c r="AK66" s="2"/>
     </row>
-    <row r="67" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -2661,7 +2662,7 @@
       <c r="AJ67" s="2"/>
       <c r="AK67" s="2"/>
     </row>
-    <row r="68" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -2688,7 +2689,7 @@
       <c r="AJ68" s="2"/>
       <c r="AK68" s="2"/>
     </row>
-    <row r="69" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -2715,7 +2716,7 @@
       <c r="AJ69" s="2"/>
       <c r="AK69" s="2"/>
     </row>
-    <row r="70" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
@@ -2742,7 +2743,7 @@
       <c r="AJ70" s="2"/>
       <c r="AK70" s="2"/>
     </row>
-    <row r="71" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
@@ -2769,7 +2770,7 @@
       <c r="AJ71" s="2"/>
       <c r="AK71" s="2"/>
     </row>
-    <row r="72" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
@@ -2796,7 +2797,7 @@
       <c r="AJ72" s="2"/>
       <c r="AK72" s="2"/>
     </row>
-    <row r="73" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -2823,7 +2824,7 @@
       <c r="AJ73" s="2"/>
       <c r="AK73" s="2"/>
     </row>
-    <row r="74" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
@@ -2850,7 +2851,7 @@
       <c r="AJ74" s="2"/>
       <c r="AK74" s="2"/>
     </row>
-    <row r="75" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="75" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -2877,7 +2878,7 @@
       <c r="AJ75" s="2"/>
       <c r="AK75" s="2"/>
     </row>
-    <row r="76" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="76" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -2904,7 +2905,7 @@
       <c r="AJ76" s="2"/>
       <c r="AK76" s="2"/>
     </row>
-    <row r="77" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="77" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -2931,7 +2932,7 @@
       <c r="AJ77" s="2"/>
       <c r="AK77" s="2"/>
     </row>
-    <row r="78" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="78" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -2958,7 +2959,7 @@
       <c r="AJ78" s="2"/>
       <c r="AK78" s="2"/>
     </row>
-    <row r="79" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="79" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -2985,7 +2986,7 @@
       <c r="AJ79" s="2"/>
       <c r="AK79" s="2"/>
     </row>
-    <row r="80" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="80" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
@@ -3012,7 +3013,7 @@
       <c r="AJ80" s="2"/>
       <c r="AK80" s="2"/>
     </row>
-    <row r="81" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="81" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
@@ -3039,7 +3040,7 @@
       <c r="AJ81" s="2"/>
       <c r="AK81" s="2"/>
     </row>
-    <row r="82" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="82" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
@@ -3066,7 +3067,7 @@
       <c r="AJ82" s="2"/>
       <c r="AK82" s="2"/>
     </row>
-    <row r="83" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="83" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
@@ -3093,7 +3094,7 @@
       <c r="AJ83" s="2"/>
       <c r="AK83" s="2"/>
     </row>
-    <row r="84" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="84" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
@@ -3120,7 +3121,7 @@
       <c r="AJ84" s="2"/>
       <c r="AK84" s="2"/>
     </row>
-    <row r="85" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="85" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
@@ -3147,7 +3148,7 @@
       <c r="AJ85" s="2"/>
       <c r="AK85" s="2"/>
     </row>
-    <row r="86" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="86" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -3174,7 +3175,7 @@
       <c r="AJ86" s="2"/>
       <c r="AK86" s="2"/>
     </row>
-    <row r="87" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="87" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
@@ -3201,7 +3202,7 @@
       <c r="AJ87" s="2"/>
       <c r="AK87" s="2"/>
     </row>
-    <row r="88" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="88" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -3228,7 +3229,7 @@
       <c r="AJ88" s="2"/>
       <c r="AK88" s="2"/>
     </row>
-    <row r="89" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="89" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
@@ -3255,7 +3256,7 @@
       <c r="AJ89" s="2"/>
       <c r="AK89" s="2"/>
     </row>
-    <row r="90" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="90" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
@@ -3282,7 +3283,7 @@
       <c r="AJ90" s="2"/>
       <c r="AK90" s="2"/>
     </row>
-    <row r="91" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="91" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
@@ -3309,7 +3310,7 @@
       <c r="AJ91" s="2"/>
       <c r="AK91" s="2"/>
     </row>
-    <row r="92" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="92" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -3336,7 +3337,7 @@
       <c r="AJ92" s="2"/>
       <c r="AK92" s="2"/>
     </row>
-    <row r="93" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="93" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -3363,7 +3364,7 @@
       <c r="AJ93" s="2"/>
       <c r="AK93" s="2"/>
     </row>
-    <row r="94" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="94" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
@@ -3390,7 +3391,7 @@
       <c r="AJ94" s="2"/>
       <c r="AK94" s="2"/>
     </row>
-    <row r="95" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="95" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
@@ -3417,7 +3418,7 @@
       <c r="AJ95" s="2"/>
       <c r="AK95" s="2"/>
     </row>
-    <row r="96" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="96" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -3444,7 +3445,7 @@
       <c r="AJ96" s="2"/>
       <c r="AK96" s="2"/>
     </row>
-    <row r="97" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="97" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -3471,7 +3472,7 @@
       <c r="AJ97" s="2"/>
       <c r="AK97" s="2"/>
     </row>
-    <row r="98" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
@@ -3498,7 +3499,7 @@
       <c r="AJ98" s="2"/>
       <c r="AK98" s="2"/>
     </row>
-    <row r="99" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="99" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
@@ -3525,7 +3526,7 @@
       <c r="AJ99" s="2"/>
       <c r="AK99" s="2"/>
     </row>
-    <row r="100" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="100" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
@@ -3552,7 +3553,7 @@
       <c r="AJ100" s="2"/>
       <c r="AK100" s="2"/>
     </row>
-    <row r="101" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="101" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
@@ -3579,7 +3580,7 @@
       <c r="AJ101" s="2"/>
       <c r="AK101" s="2"/>
     </row>
-    <row r="102" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -3606,7 +3607,7 @@
       <c r="AJ102" s="2"/>
       <c r="AK102" s="2"/>
     </row>
-    <row r="103" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="103" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
@@ -3633,7 +3634,7 @@
       <c r="AJ103" s="2"/>
       <c r="AK103" s="2"/>
     </row>
-    <row r="104" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="104" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M104" s="2"/>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -3660,7 +3661,7 @@
       <c r="AJ104" s="2"/>
       <c r="AK104" s="2"/>
     </row>
-    <row r="105" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="105" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
@@ -3687,7 +3688,7 @@
       <c r="AJ105" s="2"/>
       <c r="AK105" s="2"/>
     </row>
-    <row r="106" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="106" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
       <c r="O106" s="2"/>
@@ -3714,7 +3715,7 @@
       <c r="AJ106" s="2"/>
       <c r="AK106" s="2"/>
     </row>
-    <row r="107" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="107" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
@@ -3741,7 +3742,7 @@
       <c r="AJ107" s="2"/>
       <c r="AK107" s="2"/>
     </row>
-    <row r="108" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="108" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M108" s="2"/>
       <c r="N108" s="2"/>
       <c r="O108" s="2"/>
@@ -3768,7 +3769,7 @@
       <c r="AJ108" s="2"/>
       <c r="AK108" s="2"/>
     </row>
-    <row r="109" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="109" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M109" s="2"/>
       <c r="N109" s="2"/>
       <c r="O109" s="2"/>
@@ -3795,7 +3796,7 @@
       <c r="AJ109" s="2"/>
       <c r="AK109" s="2"/>
     </row>
-    <row r="110" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="110" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
       <c r="O110" s="2"/>
@@ -3822,7 +3823,7 @@
       <c r="AJ110" s="2"/>
       <c r="AK110" s="2"/>
     </row>
-    <row r="111" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="111" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
       <c r="O111" s="2"/>
@@ -3849,7 +3850,7 @@
       <c r="AJ111" s="2"/>
       <c r="AK111" s="2"/>
     </row>
-    <row r="112" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="112" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
       <c r="O112" s="2"/>
@@ -3876,7 +3877,7 @@
       <c r="AJ112" s="2"/>
       <c r="AK112" s="2"/>
     </row>
-    <row r="113" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
       <c r="O113" s="2"/>
@@ -3903,7 +3904,7 @@
       <c r="AJ113" s="2"/>
       <c r="AK113" s="2"/>
     </row>
-    <row r="114" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
       <c r="O114" s="2"/>
@@ -3930,7 +3931,7 @@
       <c r="AJ114" s="2"/>
       <c r="AK114" s="2"/>
     </row>
-    <row r="115" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
       <c r="O115" s="2"/>
@@ -3957,7 +3958,7 @@
       <c r="AJ115" s="2"/>
       <c r="AK115" s="2"/>
     </row>
-    <row r="116" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
       <c r="O116" s="2"/>
@@ -3984,7 +3985,7 @@
       <c r="AJ116" s="2"/>
       <c r="AK116" s="2"/>
     </row>
-    <row r="117" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="117" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
@@ -4011,7 +4012,7 @@
       <c r="AJ117" s="2"/>
       <c r="AK117" s="2"/>
     </row>
-    <row r="118" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="118" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
       <c r="O118" s="2"/>
@@ -4038,7 +4039,7 @@
       <c r="AJ118" s="2"/>
       <c r="AK118" s="2"/>
     </row>
-    <row r="119" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="119" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
       <c r="O119" s="2"/>
@@ -4065,7 +4066,7 @@
       <c r="AJ119" s="2"/>
       <c r="AK119" s="2"/>
     </row>
-    <row r="120" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="120" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M120" s="2"/>
       <c r="N120" s="2"/>
       <c r="O120" s="2"/>
@@ -4092,7 +4093,7 @@
       <c r="AJ120" s="2"/>
       <c r="AK120" s="2"/>
     </row>
-    <row r="121" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="121" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M121" s="2"/>
       <c r="N121" s="2"/>
       <c r="O121" s="2"/>
@@ -4119,7 +4120,7 @@
       <c r="AJ121" s="2"/>
       <c r="AK121" s="2"/>
     </row>
-    <row r="122" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="122" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
       <c r="O122" s="2"/>
@@ -4146,7 +4147,7 @@
       <c r="AJ122" s="2"/>
       <c r="AK122" s="2"/>
     </row>
-    <row r="123" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="123" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M123" s="2"/>
       <c r="N123" s="2"/>
       <c r="O123" s="2"/>
@@ -4173,7 +4174,7 @@
       <c r="AJ123" s="2"/>
       <c r="AK123" s="2"/>
     </row>
-    <row r="124" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="124" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M124" s="2"/>
       <c r="N124" s="2"/>
       <c r="O124" s="2"/>
@@ -4200,7 +4201,7 @@
       <c r="AJ124" s="2"/>
       <c r="AK124" s="2"/>
     </row>
-    <row r="125" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="125" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M125" s="2"/>
       <c r="N125" s="2"/>
       <c r="O125" s="2"/>
@@ -4227,7 +4228,7 @@
       <c r="AJ125" s="2"/>
       <c r="AK125" s="2"/>
     </row>
-    <row r="126" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="126" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
       <c r="O126" s="2"/>
@@ -4254,7 +4255,7 @@
       <c r="AJ126" s="2"/>
       <c r="AK126" s="2"/>
     </row>
-    <row r="127" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="127" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
       <c r="O127" s="2"/>
@@ -4281,7 +4282,7 @@
       <c r="AJ127" s="2"/>
       <c r="AK127" s="2"/>
     </row>
-    <row r="128" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="128" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M128" s="2"/>
       <c r="N128" s="2"/>
       <c r="O128" s="2"/>
@@ -4308,7 +4309,7 @@
       <c r="AJ128" s="2"/>
       <c r="AK128" s="2"/>
     </row>
-    <row r="129" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="129" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
       <c r="O129" s="2"/>
@@ -4335,7 +4336,7 @@
       <c r="AJ129" s="2"/>
       <c r="AK129" s="2"/>
     </row>
-    <row r="130" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="130" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M130" s="2"/>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
@@ -4362,7 +4363,7 @@
       <c r="AJ130" s="2"/>
       <c r="AK130" s="2"/>
     </row>
-    <row r="131" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="131" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M131" s="2"/>
       <c r="N131" s="2"/>
       <c r="O131" s="2"/>
@@ -4389,7 +4390,7 @@
       <c r="AJ131" s="2"/>
       <c r="AK131" s="2"/>
     </row>
-    <row r="132" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="132" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M132" s="2"/>
       <c r="N132" s="2"/>
       <c r="O132" s="2"/>
@@ -4416,7 +4417,7 @@
       <c r="AJ132" s="2"/>
       <c r="AK132" s="2"/>
     </row>
-    <row r="133" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="133" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M133" s="2"/>
       <c r="N133" s="2"/>
       <c r="O133" s="2"/>
@@ -4443,7 +4444,7 @@
       <c r="AJ133" s="2"/>
       <c r="AK133" s="2"/>
     </row>
-    <row r="134" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="134" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M134" s="2"/>
       <c r="N134" s="2"/>
       <c r="O134" s="2"/>
@@ -4470,7 +4471,7 @@
       <c r="AJ134" s="2"/>
       <c r="AK134" s="2"/>
     </row>
-    <row r="135" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="135" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M135" s="2"/>
       <c r="N135" s="2"/>
       <c r="O135" s="2"/>
@@ -4497,7 +4498,7 @@
       <c r="AJ135" s="2"/>
       <c r="AK135" s="2"/>
     </row>
-    <row r="136" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="136" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M136" s="2"/>
       <c r="N136" s="2"/>
       <c r="O136" s="2"/>
@@ -4524,7 +4525,7 @@
       <c r="AJ136" s="2"/>
       <c r="AK136" s="2"/>
     </row>
-    <row r="137" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="137" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M137" s="2"/>
       <c r="N137" s="2"/>
       <c r="O137" s="2"/>
@@ -4551,7 +4552,7 @@
       <c r="AJ137" s="2"/>
       <c r="AK137" s="2"/>
     </row>
-    <row r="138" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="138" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M138" s="2"/>
       <c r="N138" s="2"/>
       <c r="O138" s="2"/>
@@ -4578,7 +4579,7 @@
       <c r="AJ138" s="2"/>
       <c r="AK138" s="2"/>
     </row>
-    <row r="139" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="139" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M139" s="2"/>
       <c r="N139" s="2"/>
       <c r="O139" s="2"/>
@@ -4605,7 +4606,7 @@
       <c r="AJ139" s="2"/>
       <c r="AK139" s="2"/>
     </row>
-    <row r="140" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="140" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M140" s="2"/>
       <c r="N140" s="2"/>
       <c r="O140" s="2"/>
@@ -4632,7 +4633,7 @@
       <c r="AJ140" s="2"/>
       <c r="AK140" s="2"/>
     </row>
-    <row r="141" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="141" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M141" s="2"/>
       <c r="N141" s="2"/>
       <c r="O141" s="2"/>
@@ -4659,7 +4660,7 @@
       <c r="AJ141" s="2"/>
       <c r="AK141" s="2"/>
     </row>
-    <row r="142" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="142" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M142" s="2"/>
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
@@ -4686,7 +4687,7 @@
       <c r="AJ142" s="2"/>
       <c r="AK142" s="2"/>
     </row>
-    <row r="143" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="143" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M143" s="2"/>
       <c r="N143" s="2"/>
       <c r="O143" s="2"/>
@@ -4713,7 +4714,7 @@
       <c r="AJ143" s="2"/>
       <c r="AK143" s="2"/>
     </row>
-    <row r="144" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="144" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M144" s="2"/>
       <c r="N144" s="2"/>
       <c r="O144" s="2"/>
@@ -4740,7 +4741,7 @@
       <c r="AJ144" s="2"/>
       <c r="AK144" s="2"/>
     </row>
-    <row r="145" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="145" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M145" s="2"/>
       <c r="N145" s="2"/>
       <c r="O145" s="2"/>
@@ -4767,7 +4768,7 @@
       <c r="AJ145" s="2"/>
       <c r="AK145" s="2"/>
     </row>
-    <row r="146" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="146" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
@@ -4794,7 +4795,7 @@
       <c r="AJ146" s="2"/>
       <c r="AK146" s="2"/>
     </row>
-    <row r="147" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="147" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M147" s="2"/>
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
@@ -4821,7 +4822,7 @@
       <c r="AJ147" s="2"/>
       <c r="AK147" s="2"/>
     </row>
-    <row r="148" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="148" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
       <c r="O148" s="2"/>
@@ -4848,7 +4849,7 @@
       <c r="AJ148" s="2"/>
       <c r="AK148" s="2"/>
     </row>
-    <row r="149" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="149" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
@@ -4875,7 +4876,7 @@
       <c r="AJ149" s="2"/>
       <c r="AK149" s="2"/>
     </row>
-    <row r="150" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="150" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
       <c r="O150" s="2"/>
@@ -4902,7 +4903,7 @@
       <c r="AJ150" s="2"/>
       <c r="AK150" s="2"/>
     </row>
-    <row r="151" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="151" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M151" s="2"/>
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
@@ -4929,7 +4930,7 @@
       <c r="AJ151" s="2"/>
       <c r="AK151" s="2"/>
     </row>
-    <row r="152" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="152" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M152" s="2"/>
       <c r="N152" s="2"/>
       <c r="O152" s="2"/>
@@ -4956,7 +4957,7 @@
       <c r="AJ152" s="2"/>
       <c r="AK152" s="2"/>
     </row>
-    <row r="153" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="153" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M153" s="2"/>
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
@@ -4983,7 +4984,7 @@
       <c r="AJ153" s="2"/>
       <c r="AK153" s="2"/>
     </row>
-    <row r="154" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="154" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
       <c r="O154" s="2"/>
@@ -5010,7 +5011,7 @@
       <c r="AJ154" s="2"/>
       <c r="AK154" s="2"/>
     </row>
-    <row r="155" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="155" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M155" s="2"/>
       <c r="N155" s="2"/>
       <c r="O155" s="2"/>
@@ -5037,7 +5038,7 @@
       <c r="AJ155" s="2"/>
       <c r="AK155" s="2"/>
     </row>
-    <row r="156" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="156" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
       <c r="O156" s="2"/>
@@ -5064,7 +5065,7 @@
       <c r="AJ156" s="2"/>
       <c r="AK156" s="2"/>
     </row>
-    <row r="157" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="157" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
       <c r="O157" s="2"/>
@@ -5091,7 +5092,7 @@
       <c r="AJ157" s="2"/>
       <c r="AK157" s="2"/>
     </row>
-    <row r="158" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="158" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M158" s="2"/>
       <c r="N158" s="2"/>
       <c r="O158" s="2"/>
@@ -5118,7 +5119,7 @@
       <c r="AJ158" s="2"/>
       <c r="AK158" s="2"/>
     </row>
-    <row r="159" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="159" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M159" s="2"/>
       <c r="N159" s="2"/>
       <c r="O159" s="2"/>
@@ -5145,7 +5146,7 @@
       <c r="AJ159" s="2"/>
       <c r="AK159" s="2"/>
     </row>
-    <row r="160" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="160" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M160" s="2"/>
       <c r="N160" s="2"/>
       <c r="O160" s="2"/>
@@ -5172,7 +5173,7 @@
       <c r="AJ160" s="2"/>
       <c r="AK160" s="2"/>
     </row>
-    <row r="161" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="161" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
       <c r="O161" s="2"/>
@@ -5201,13 +5202,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A15:C18"/>
     <mergeCell ref="D15:F18"/>
     <mergeCell ref="G15:I18"/>
@@ -5221,6 +5215,13 @@
     <mergeCell ref="D11:F14"/>
     <mergeCell ref="G11:I14"/>
     <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5228,21 +5229,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008EA8F6205B617B4CBD762DBD6D300502" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="000a41c94a85e4495c2f2d3453c30ed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10b95d85-a823-4616-89f6-0a6587d88b0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0729d4038857d2ede91d1e28869f4e90" ns3:_="">
     <xsd:import namespace="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
@@ -5388,31 +5374,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A39B317-7C09-4361-8F9C-EC6B55EB4D12}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5428,4 +5405,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>